<commit_message>
add dynamic beammasking, filtering
</commit_message>
<xml_diff>
--- a/doc/firmware-register-map.xlsx
+++ b/doc/firmware-register-map.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eric\Desktop\firmware-proto-beacon\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eric\Desktop\firmware-proto-beacon\firmware-proto-beacon\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21384" windowHeight="7140"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21390" windowHeight="7140"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="225">
   <si>
     <t>Register Map</t>
   </si>
@@ -479,12 +479,6 @@
     <t>external trigger input config</t>
   </si>
   <si>
-    <t>x000700</t>
-  </si>
-  <si>
-    <t>x0001FF</t>
-  </si>
-  <si>
     <t>if LSB=0, ext trig input acts as 'gate only' for scalers</t>
   </si>
   <si>
@@ -657,12 +651,60 @@
   </si>
   <si>
     <t>24 bit counter of pps pulses</t>
+  </si>
+  <si>
+    <t>x000300</t>
+  </si>
+  <si>
+    <t>low pass filter register</t>
+  </si>
+  <si>
+    <t>LSB enable ; bit 8 enables filtered data to data manager (otherwise nonfiltered data saved)</t>
+  </si>
+  <si>
+    <t>x0000FF</t>
+  </si>
+  <si>
+    <t>low pass filter register (2)</t>
+  </si>
+  <si>
+    <t>x000005</t>
+  </si>
+  <si>
+    <t>lower 8 bits = post filter bitshift (division)</t>
+  </si>
+  <si>
+    <t>dynamic beam mask register</t>
+  </si>
+  <si>
+    <t>lower 8 bits [0..7]=&gt; threshold ; bit 8 =&gt; enable/disable</t>
+  </si>
+  <si>
+    <t>x000105</t>
+  </si>
+  <si>
+    <t>dynamic beam mask register (2)</t>
+  </si>
+  <si>
+    <t>lower 8 bits [0..7]=&gt; mask holdoff length</t>
+  </si>
+  <si>
+    <t>x000040</t>
+  </si>
+  <si>
+    <t>metadata-&gt; dynamic beam mask</t>
+  </si>
+  <si>
+    <t>24 bit dynamic beam mask</t>
+  </si>
+  <si>
+    <t>dynamic beam mask value</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -724,7 +766,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -801,17 +843,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -851,9 +882,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -887,12 +915,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1175,69 +1204,69 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D11" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.88671875" customWidth="1"/>
-    <col min="2" max="2" width="8.44140625" style="13" customWidth="1"/>
-    <col min="3" max="3" width="60.33203125" customWidth="1"/>
-    <col min="4" max="4" width="82.44140625" customWidth="1"/>
-    <col min="5" max="5" width="23.44140625" customWidth="1"/>
-    <col min="6" max="6" width="74.88671875" style="5" customWidth="1"/>
-    <col min="7" max="7" width="7.44140625" customWidth="1"/>
+    <col min="1" max="1" width="4.85546875" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" style="13" customWidth="1"/>
+    <col min="3" max="3" width="60.28515625" customWidth="1"/>
+    <col min="4" max="4" width="82.42578125" customWidth="1"/>
+    <col min="5" max="5" width="23.42578125" customWidth="1"/>
+    <col min="6" max="6" width="74.85546875" style="5" customWidth="1"/>
+    <col min="7" max="7" width="7.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="39" t="s">
-        <v>172</v>
-      </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="39" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="41" t="s">
+        <v>170</v>
+      </c>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="39" t="s">
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
       <c r="F3" s="6"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="40">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="42">
         <v>43305</v>
       </c>
-      <c r="B4" s="41"/>
+      <c r="B4" s="43"/>
       <c r="C4" s="1"/>
       <c r="D4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -1256,27 +1285,27 @@
       <c r="F6" s="7"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0</v>
       </c>
-      <c r="B7" s="27" t="str">
+      <c r="B7" s="26" t="str">
         <f>"x" &amp; DEC2HEX(A7,2)</f>
         <v>x00</v>
       </c>
       <c r="C7" t="s">
         <v>93</v>
       </c>
-      <c r="D7" s="26" t="s">
+      <c r="D7" s="25" t="s">
         <v>95</v>
       </c>
       <c r="F7" s="13"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
-      <c r="B8" s="27" t="str">
+      <c r="B8" s="26" t="str">
         <f t="shared" ref="B8:B71" si="0">"x" &amp; DEC2HEX(A8,2)</f>
         <v>x01</v>
       </c>
@@ -1287,12 +1316,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <f>1+A8</f>
         <v>2</v>
       </c>
-      <c r="B9" s="27" t="str">
+      <c r="B9" s="26" t="str">
         <f t="shared" si="0"/>
         <v>x02</v>
       </c>
@@ -1303,12 +1332,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" ref="A10:A73" si="1">1+A9</f>
         <v>3</v>
       </c>
-      <c r="B10" s="27" t="str">
+      <c r="B10" s="26" t="str">
         <f t="shared" si="0"/>
         <v>x03</v>
       </c>
@@ -1322,12 +1351,12 @@
         <v>111</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="B11" s="27" t="str">
+      <c r="B11" s="26" t="str">
         <f t="shared" si="0"/>
         <v>x04</v>
       </c>
@@ -1341,12 +1370,12 @@
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="B12" s="27" t="str">
+      <c r="B12" s="26" t="str">
         <f t="shared" si="0"/>
         <v>x05</v>
       </c>
@@ -1360,12 +1389,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="B13" s="27" t="str">
+      <c r="B13" s="26" t="str">
         <f t="shared" si="0"/>
         <v>x06</v>
       </c>
@@ -1379,12 +1408,12 @@
         <v>118</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="B14" s="27" t="str">
+      <c r="B14" s="26" t="str">
         <f t="shared" si="0"/>
         <v>x07</v>
       </c>
@@ -1398,12 +1427,12 @@
         <v>92</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="B15" s="27" t="str">
+      <c r="B15" s="26" t="str">
         <f t="shared" si="0"/>
         <v>x08</v>
       </c>
@@ -1417,12 +1446,12 @@
         <v>91</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="B16" s="27" t="str">
+      <c r="B16" s="26" t="str">
         <f t="shared" si="0"/>
         <v>x09</v>
       </c>
@@ -1433,12 +1462,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="14">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="B17" s="28" t="str">
+      <c r="B17" s="27" t="str">
         <f t="shared" si="0"/>
         <v>x0A</v>
       </c>
@@ -1455,12 +1484,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="17">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="B18" s="29" t="str">
+      <c r="B18" s="28" t="str">
         <f t="shared" si="0"/>
         <v>x0B</v>
       </c>
@@ -1475,12 +1504,12 @@
       </c>
       <c r="F18" s="19"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="17">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="B19" s="29" t="str">
+      <c r="B19" s="28" t="str">
         <f t="shared" si="0"/>
         <v>x0C</v>
       </c>
@@ -1495,12 +1524,12 @@
       </c>
       <c r="F19" s="19"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="17">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="B20" s="29" t="str">
+      <c r="B20" s="28" t="str">
         <f t="shared" si="0"/>
         <v>x0D</v>
       </c>
@@ -1515,12 +1544,12 @@
       </c>
       <c r="F20" s="19"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="17">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="B21" s="29" t="str">
+      <c r="B21" s="28" t="str">
         <f t="shared" si="0"/>
         <v>x0E</v>
       </c>
@@ -1535,12 +1564,12 @@
       </c>
       <c r="F21" s="19"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="17">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="B22" s="29" t="str">
+      <c r="B22" s="28" t="str">
         <f t="shared" si="0"/>
         <v>x0F</v>
       </c>
@@ -1555,12 +1584,12 @@
       </c>
       <c r="F22" s="19"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="17">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="B23" s="29" t="str">
+      <c r="B23" s="28" t="str">
         <f t="shared" si="0"/>
         <v>x10</v>
       </c>
@@ -1577,17 +1606,17 @@
         <v>103</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="17">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="B24" s="29" t="str">
+      <c r="B24" s="28" t="str">
         <f t="shared" si="0"/>
         <v>x11</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D24" s="18" t="s">
         <v>61</v>
@@ -1596,15 +1625,15 @@
         <v>6</v>
       </c>
       <c r="F24" s="19" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="17">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="B25" s="29" t="str">
+      <c r="B25" s="28" t="str">
         <f t="shared" si="0"/>
         <v>x12</v>
       </c>
@@ -1618,15 +1647,15 @@
         <v>6</v>
       </c>
       <c r="F25" s="19" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="17">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="B26" s="29" t="str">
+      <c r="B26" s="28" t="str">
         <f t="shared" si="0"/>
         <v>x13</v>
       </c>
@@ -1641,17 +1670,17 @@
       </c>
       <c r="F26" s="19"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="17">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="B27" s="29" t="str">
+      <c r="B27" s="28" t="str">
         <f t="shared" si="0"/>
         <v>x14</v>
       </c>
-      <c r="C27" s="23" t="s">
-        <v>166</v>
+      <c r="C27" s="22" t="s">
+        <v>164</v>
       </c>
       <c r="D27" s="18" t="s">
         <v>61</v>
@@ -1660,20 +1689,20 @@
         <v>6</v>
       </c>
       <c r="F27" s="19" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="17">
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="B28" s="29" t="str">
+      <c r="B28" s="28" t="str">
         <f t="shared" si="0"/>
         <v>x15</v>
       </c>
-      <c r="C28" s="23" t="s">
-        <v>168</v>
+      <c r="C28" s="22" t="s">
+        <v>166</v>
       </c>
       <c r="D28" s="18" t="s">
         <v>61</v>
@@ -1682,53 +1711,59 @@
         <v>6</v>
       </c>
       <c r="F28" s="19" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="17">
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="B29" s="29" t="str">
+      <c r="B29" s="28" t="str">
         <f t="shared" si="0"/>
         <v>x16</v>
       </c>
-      <c r="C29" s="23" t="s">
-        <v>209</v>
-      </c>
-      <c r="D29" s="23" t="s">
+      <c r="C29" s="22" t="s">
+        <v>207</v>
+      </c>
+      <c r="D29" s="22" t="s">
         <v>61</v>
       </c>
       <c r="E29" s="18" t="s">
         <v>6</v>
       </c>
       <c r="F29" s="19" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="17">
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="B30" s="29" t="str">
+      <c r="B30" s="28" t="str">
         <f t="shared" si="0"/>
         <v>x17</v>
       </c>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
+      <c r="C30" s="22" t="s">
+        <v>222</v>
+      </c>
+      <c r="D30" s="22" t="s">
+        <v>61</v>
+      </c>
       <c r="E30" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="F30" s="19"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F30" s="19" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="17">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="B31" s="29" t="str">
+      <c r="B31" s="28" t="str">
         <f t="shared" si="0"/>
         <v>x18</v>
       </c>
@@ -1739,12 +1774,12 @@
       </c>
       <c r="F31" s="19"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="17">
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="B32" s="29" t="str">
+      <c r="B32" s="28" t="str">
         <f t="shared" si="0"/>
         <v>x19</v>
       </c>
@@ -1755,12 +1790,12 @@
       </c>
       <c r="F32" s="19"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="17">
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="B33" s="29" t="str">
+      <c r="B33" s="28" t="str">
         <f t="shared" si="0"/>
         <v>x1A</v>
       </c>
@@ -1771,12 +1806,12 @@
       </c>
       <c r="F33" s="19"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="17">
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="B34" s="29" t="str">
+      <c r="B34" s="28" t="str">
         <f t="shared" si="0"/>
         <v>x1B</v>
       </c>
@@ -1787,12 +1822,12 @@
       </c>
       <c r="F34" s="19"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="17">
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="B35" s="29" t="str">
+      <c r="B35" s="28" t="str">
         <f t="shared" si="0"/>
         <v>x1C</v>
       </c>
@@ -1803,12 +1838,12 @@
       </c>
       <c r="F35" s="19"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="17">
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="B36" s="29" t="str">
+      <c r="B36" s="28" t="str">
         <f t="shared" si="0"/>
         <v>x1D</v>
       </c>
@@ -1819,12 +1854,12 @@
       </c>
       <c r="F36" s="19"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="17">
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="B37" s="29" t="str">
+      <c r="B37" s="28" t="str">
         <f t="shared" si="0"/>
         <v>x1E</v>
       </c>
@@ -1835,12 +1870,12 @@
       </c>
       <c r="F37" s="19"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="17">
         <f t="shared" si="1"/>
         <v>31</v>
       </c>
-      <c r="B38" s="29" t="str">
+      <c r="B38" s="28" t="str">
         <f t="shared" si="0"/>
         <v>x1F</v>
       </c>
@@ -1851,12 +1886,12 @@
       </c>
       <c r="F38" s="19"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="17">
         <f t="shared" si="1"/>
         <v>32</v>
       </c>
-      <c r="B39" s="29" t="str">
+      <c r="B39" s="28" t="str">
         <f t="shared" si="0"/>
         <v>x20</v>
       </c>
@@ -1867,12 +1902,12 @@
       </c>
       <c r="F39" s="19"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="17">
         <f t="shared" si="1"/>
         <v>33</v>
       </c>
-      <c r="B40" s="29" t="str">
+      <c r="B40" s="28" t="str">
         <f t="shared" si="0"/>
         <v>x21</v>
       </c>
@@ -1883,111 +1918,117 @@
       </c>
       <c r="F40" s="19"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="20">
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
-      <c r="B41" s="30" t="str">
+      <c r="B41" s="29" t="str">
         <f t="shared" si="0"/>
         <v>x22</v>
       </c>
-      <c r="C41" s="21"/>
-      <c r="D41" s="21"/>
+      <c r="C41" s="21" t="s">
+        <v>224</v>
+      </c>
+      <c r="D41" s="38" t="s">
+        <v>15</v>
+      </c>
       <c r="E41" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="F41" s="22"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F41" s="19" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
-      <c r="B42" s="27" t="str">
+      <c r="B42" s="26" t="str">
         <f t="shared" si="0"/>
         <v>x23</v>
       </c>
-      <c r="C42" s="23" t="s">
+      <c r="C42" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="D42" s="23" t="s">
+      <c r="D42" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="F42" s="24" t="s">
+      <c r="F42" s="23" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-      <c r="B43" s="27" t="str">
+      <c r="B43" s="26" t="str">
         <f t="shared" si="0"/>
         <v>x24</v>
       </c>
-      <c r="C43" s="23" t="s">
+      <c r="C43" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="D43" s="23" t="s">
+      <c r="D43" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="F43" s="24" t="s">
+      <c r="F43" s="23" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44">
         <f t="shared" si="1"/>
         <v>37</v>
       </c>
-      <c r="B44" s="27" t="str">
+      <c r="B44" s="26" t="str">
         <f t="shared" si="0"/>
         <v>x25</v>
       </c>
-      <c r="C44" s="23" t="s">
+      <c r="C44" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="D44" s="23" t="s">
+      <c r="D44" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="F44" s="24" t="s">
+      <c r="F44" s="23" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
         <f t="shared" si="1"/>
         <v>38</v>
       </c>
-      <c r="B45" s="27" t="str">
+      <c r="B45" s="26" t="str">
         <f t="shared" si="0"/>
         <v>x26</v>
       </c>
-      <c r="C45" s="23" t="s">
+      <c r="C45" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="D45" s="23" t="s">
+      <c r="D45" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="F45" s="24" t="s">
+      <c r="F45" s="23" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
         <f t="shared" si="1"/>
         <v>39</v>
       </c>
-      <c r="B46" s="27" t="str">
+      <c r="B46" s="26" t="str">
         <f t="shared" si="0"/>
         <v>x27</v>
       </c>
-      <c r="C46" s="23" t="s">
+      <c r="C46" s="22" t="s">
         <v>99</v>
       </c>
-      <c r="D46" s="23" t="s">
+      <c r="D46" s="22" t="s">
         <v>101</v>
       </c>
       <c r="E46" t="s">
@@ -1997,31 +2038,31 @@
         <v>100</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47">
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="B47" s="27" t="str">
+      <c r="B47" s="26" t="str">
         <f t="shared" si="0"/>
         <v>x28</v>
       </c>
       <c r="C47" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D47" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E47" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A48">
         <f t="shared" si="1"/>
         <v>41</v>
       </c>
-      <c r="B48" s="27" t="str">
+      <c r="B48" s="26" t="str">
         <f t="shared" si="0"/>
         <v>x29</v>
       </c>
@@ -2029,21 +2070,21 @@
         <v>58</v>
       </c>
       <c r="D48" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E48" t="s">
         <v>6</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49">
         <f t="shared" si="1"/>
         <v>42</v>
       </c>
-      <c r="B49" s="27" t="str">
+      <c r="B49" s="26" t="str">
         <f t="shared" si="0"/>
         <v>x2A</v>
       </c>
@@ -2060,80 +2101,80 @@
         <v>40</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50">
         <f t="shared" si="1"/>
         <v>43</v>
       </c>
-      <c r="B50" s="27" t="str">
+      <c r="B50" s="26" t="str">
         <f t="shared" si="0"/>
         <v>x2B</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51">
         <f t="shared" si="1"/>
         <v>44</v>
       </c>
-      <c r="B51" s="27" t="str">
+      <c r="B51" s="26" t="str">
         <f t="shared" si="0"/>
         <v>x2C</v>
       </c>
       <c r="C51" t="s">
+        <v>156</v>
+      </c>
+      <c r="D51" t="s">
+        <v>159</v>
+      </c>
+      <c r="F51" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="D51" t="s">
-        <v>161</v>
-      </c>
-      <c r="F51" s="5" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52">
         <f t="shared" si="1"/>
         <v>45</v>
       </c>
-      <c r="B52" s="27" t="str">
+      <c r="B52" s="26" t="str">
         <f t="shared" si="0"/>
         <v>x2D</v>
       </c>
-      <c r="C52" s="33" t="s">
+      <c r="C52" s="32" t="s">
+        <v>157</v>
+      </c>
+      <c r="D52" s="32" t="s">
         <v>159</v>
       </c>
-      <c r="D52" s="33" t="s">
-        <v>161</v>
-      </c>
       <c r="F52" s="5" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53">
         <f t="shared" si="1"/>
         <v>46</v>
       </c>
-      <c r="B53" s="27" t="str">
+      <c r="B53" s="26" t="str">
         <f t="shared" si="0"/>
         <v>x2E</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54">
         <f t="shared" si="1"/>
         <v>47</v>
       </c>
-      <c r="B54" s="27" t="str">
+      <c r="B54" s="26" t="str">
         <f t="shared" si="0"/>
         <v>x2F</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55">
         <f t="shared" si="1"/>
         <v>48</v>
       </c>
-      <c r="B55" s="27" t="str">
+      <c r="B55" s="26" t="str">
         <f t="shared" si="0"/>
         <v>x30</v>
       </c>
@@ -2150,22 +2191,22 @@
         <v>113</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56">
         <f t="shared" si="1"/>
         <v>49</v>
       </c>
-      <c r="B56" s="27" t="str">
+      <c r="B56" s="26" t="str">
         <f t="shared" si="0"/>
         <v>x31</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57">
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="B57" s="27" t="str">
+      <c r="B57" s="26" t="str">
         <f t="shared" si="0"/>
         <v>x32</v>
       </c>
@@ -2182,12 +2223,12 @@
         <v>112</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58">
         <f t="shared" si="1"/>
         <v>51</v>
       </c>
-      <c r="B58" s="27" t="str">
+      <c r="B58" s="26" t="str">
         <f t="shared" si="0"/>
         <v>x33</v>
       </c>
@@ -2204,12 +2245,12 @@
         <v>112</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59">
         <f t="shared" si="1"/>
         <v>52</v>
       </c>
-      <c r="B59" s="27" t="str">
+      <c r="B59" s="26" t="str">
         <f t="shared" si="0"/>
         <v>x34</v>
       </c>
@@ -2226,12 +2267,12 @@
         <v>112</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60">
         <f t="shared" si="1"/>
         <v>53</v>
       </c>
-      <c r="B60" s="27" t="str">
+      <c r="B60" s="26" t="str">
         <f t="shared" si="0"/>
         <v>x35</v>
       </c>
@@ -2245,22 +2286,22 @@
         <v>6</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61">
         <f t="shared" si="1"/>
         <v>54</v>
       </c>
-      <c r="B61" s="27" t="str">
+      <c r="B61" s="26" t="str">
         <f t="shared" si="0"/>
         <v>x36</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62">
         <f t="shared" si="1"/>
         <v>55</v>
       </c>
-      <c r="B62" s="27" t="str">
+      <c r="B62" s="26" t="str">
         <f t="shared" si="0"/>
         <v>x37</v>
       </c>
@@ -2274,12 +2315,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A63">
         <f t="shared" si="1"/>
         <v>56</v>
       </c>
-      <c r="B63" s="27" t="str">
+      <c r="B63" s="26" t="str">
         <f t="shared" si="0"/>
         <v>x38</v>
       </c>
@@ -2293,12 +2334,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A64">
         <f t="shared" si="1"/>
         <v>57</v>
       </c>
-      <c r="B64" s="27" t="str">
+      <c r="B64" s="26" t="str">
         <f t="shared" si="0"/>
         <v>x39</v>
       </c>
@@ -2312,12 +2353,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A65">
         <f t="shared" si="1"/>
         <v>58</v>
       </c>
-      <c r="B65" s="27" t="str">
+      <c r="B65" s="26" t="str">
         <f t="shared" si="0"/>
         <v>x3A</v>
       </c>
@@ -2331,12 +2372,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A66">
         <f t="shared" si="1"/>
         <v>59</v>
       </c>
-      <c r="B66" s="27" t="str">
+      <c r="B66" s="26" t="str">
         <f t="shared" si="0"/>
         <v>x3B</v>
       </c>
@@ -2350,12 +2391,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67">
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
-      <c r="B67" s="27" t="str">
+      <c r="B67" s="26" t="str">
         <f t="shared" si="0"/>
         <v>x3C</v>
       </c>
@@ -2369,47 +2410,47 @@
         <v>6</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68">
         <f t="shared" si="1"/>
         <v>61</v>
       </c>
-      <c r="B68" s="27" t="str">
+      <c r="B68" s="26" t="str">
         <f t="shared" si="0"/>
         <v>x3D</v>
       </c>
       <c r="D68" s="5"/>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69">
         <f t="shared" si="1"/>
         <v>62</v>
       </c>
-      <c r="B69" s="27" t="str">
+      <c r="B69" s="26" t="str">
         <f t="shared" si="0"/>
         <v>x3E</v>
       </c>
-      <c r="C69" s="35"/>
+      <c r="C69" s="34"/>
       <c r="D69" s="5"/>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70">
         <f t="shared" si="1"/>
         <v>63</v>
       </c>
-      <c r="B70" s="27" t="str">
+      <c r="B70" s="26" t="str">
         <f t="shared" si="0"/>
         <v>x3F</v>
       </c>
-      <c r="C70" s="35"/>
+      <c r="C70" s="34"/>
       <c r="D70" s="5"/>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71">
         <f t="shared" si="1"/>
         <v>64</v>
       </c>
-      <c r="B71" s="27" t="str">
+      <c r="B71" s="26" t="str">
         <f t="shared" si="0"/>
         <v>x40</v>
       </c>
@@ -2423,12 +2464,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72">
         <f t="shared" si="1"/>
         <v>65</v>
       </c>
-      <c r="B72" s="27" t="str">
+      <c r="B72" s="26" t="str">
         <f t="shared" ref="B72:B135" si="2">"x" &amp; DEC2HEX(A72,2)</f>
         <v>x41</v>
       </c>
@@ -2442,12 +2483,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73">
         <f t="shared" si="1"/>
         <v>66</v>
       </c>
-      <c r="B73" s="27" t="str">
+      <c r="B73" s="26" t="str">
         <f t="shared" si="2"/>
         <v>x42</v>
       </c>
@@ -2464,34 +2505,34 @@
         <v>46</v>
       </c>
     </row>
-    <row r="74" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="8">
         <f t="shared" ref="A74:A134" si="3">1+A73</f>
         <v>67</v>
       </c>
-      <c r="B74" s="27" t="str">
+      <c r="B74" s="26" t="str">
         <f t="shared" si="2"/>
         <v>x43</v>
       </c>
       <c r="F74" s="10"/>
     </row>
-    <row r="75" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="8">
         <f t="shared" si="3"/>
         <v>68</v>
       </c>
-      <c r="B75" s="27" t="str">
+      <c r="B75" s="26" t="str">
         <f t="shared" si="2"/>
         <v>x44</v>
       </c>
       <c r="F75" s="10"/>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="8">
         <f t="shared" si="3"/>
         <v>69</v>
       </c>
-      <c r="B76" s="27" t="str">
+      <c r="B76" s="26" t="str">
         <f t="shared" si="2"/>
         <v>x45</v>
       </c>
@@ -2508,23 +2549,23 @@
         <v>89</v>
       </c>
     </row>
-    <row r="77" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="8">
         <f t="shared" si="3"/>
         <v>70</v>
       </c>
-      <c r="B77" s="27" t="str">
+      <c r="B77" s="26" t="str">
         <f t="shared" si="2"/>
         <v>x46</v>
       </c>
       <c r="F77" s="10"/>
     </row>
-    <row r="78" spans="1:6" s="9" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" s="8">
         <f t="shared" si="3"/>
         <v>71</v>
       </c>
-      <c r="B78" s="27" t="str">
+      <c r="B78" s="26" t="str">
         <f t="shared" si="2"/>
         <v>x47</v>
       </c>
@@ -2541,12 +2582,12 @@
         <v>96</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="8">
         <f t="shared" si="3"/>
         <v>72</v>
       </c>
-      <c r="B79" s="27" t="str">
+      <c r="B79" s="26" t="str">
         <f t="shared" si="2"/>
         <v>x48</v>
       </c>
@@ -2559,27 +2600,27 @@
       <c r="E79" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="F79" s="25" t="s">
+      <c r="F79" s="24" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="8">
         <f t="shared" si="3"/>
         <v>73</v>
       </c>
-      <c r="B80" s="27" t="str">
+      <c r="B80" s="26" t="str">
         <f t="shared" si="2"/>
         <v>x49</v>
       </c>
       <c r="E80" s="4"/>
     </row>
-    <row r="81" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="8">
         <f t="shared" si="3"/>
         <v>74</v>
       </c>
-      <c r="B81" s="27" t="str">
+      <c r="B81" s="26" t="str">
         <f t="shared" si="2"/>
         <v>x4A</v>
       </c>
@@ -2587,34 +2628,34 @@
       <c r="D81" s="12"/>
       <c r="F81" s="10"/>
     </row>
-    <row r="82" spans="1:6" s="9" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:6" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="8">
         <f t="shared" si="3"/>
         <v>75</v>
       </c>
-      <c r="B82" s="27" t="str">
+      <c r="B82" s="26" t="str">
         <f t="shared" si="2"/>
         <v>x4B</v>
       </c>
       <c r="C82" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="D82" s="25" t="s">
-        <v>154</v>
+      <c r="D82" s="24" t="s">
+        <v>152</v>
       </c>
       <c r="E82" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="F82" s="34" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="83" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F82" s="33" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A83">
         <f t="shared" si="3"/>
         <v>76</v>
       </c>
-      <c r="B83" s="27" t="str">
+      <c r="B83" s="26" t="str">
         <f t="shared" si="2"/>
         <v>x4C</v>
       </c>
@@ -2622,7 +2663,7 @@
         <v>50</v>
       </c>
       <c r="D83" s="5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E83" t="s">
         <v>114</v>
@@ -2631,12 +2672,12 @@
         <v>115</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84">
         <f t="shared" si="3"/>
         <v>77</v>
       </c>
-      <c r="B84" s="27" t="str">
+      <c r="B84" s="26" t="str">
         <f t="shared" si="2"/>
         <v>x4D</v>
       </c>
@@ -2653,12 +2694,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85">
         <f t="shared" si="3"/>
         <v>78</v>
       </c>
-      <c r="B85" s="27" t="str">
+      <c r="B85" s="26" t="str">
         <f t="shared" si="2"/>
         <v>x4E</v>
       </c>
@@ -2675,31 +2716,31 @@
         <v>77</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86">
         <f t="shared" si="3"/>
         <v>79</v>
       </c>
-      <c r="B86" s="27" t="str">
+      <c r="B86" s="26" t="str">
         <f t="shared" si="2"/>
         <v>x4F</v>
       </c>
       <c r="C86" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D86" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E86" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87">
         <f t="shared" si="3"/>
         <v>80</v>
       </c>
-      <c r="B87" s="27" t="str">
+      <c r="B87" s="26" t="str">
         <f t="shared" si="2"/>
         <v>x50</v>
       </c>
@@ -2716,12 +2757,12 @@
         <v>48</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88">
         <f t="shared" si="3"/>
         <v>81</v>
       </c>
-      <c r="B88" s="27" t="str">
+      <c r="B88" s="26" t="str">
         <f t="shared" si="2"/>
         <v>x51</v>
       </c>
@@ -2732,18 +2773,18 @@
         <v>122</v>
       </c>
       <c r="E88" t="s">
-        <v>152</v>
+        <v>212</v>
       </c>
       <c r="F88" s="5" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89">
         <f t="shared" si="3"/>
         <v>82</v>
       </c>
-      <c r="B89" s="27" t="str">
+      <c r="B89" s="26" t="str">
         <f t="shared" si="2"/>
         <v>x52</v>
       </c>
@@ -2751,21 +2792,21 @@
         <v>149</v>
       </c>
       <c r="D89" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E89" t="s">
-        <v>151</v>
+        <v>209</v>
       </c>
       <c r="F89" s="5" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="90" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A90">
         <f t="shared" si="3"/>
         <v>83</v>
       </c>
-      <c r="B90" s="27" t="str">
+      <c r="B90" s="26" t="str">
         <f t="shared" si="2"/>
         <v>x53</v>
       </c>
@@ -2773,21 +2814,21 @@
         <v>98</v>
       </c>
       <c r="D90" s="5" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E90" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F90" s="5" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A91">
         <f t="shared" si="3"/>
         <v>84</v>
       </c>
-      <c r="B91" s="27" t="str">
+      <c r="B91" s="26" t="str">
         <f t="shared" si="2"/>
         <v>x54</v>
       </c>
@@ -2804,12 +2845,12 @@
         <v>110</v>
       </c>
     </row>
-    <row r="92" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A92">
         <f t="shared" si="3"/>
         <v>85</v>
       </c>
-      <c r="B92" s="27" t="str">
+      <c r="B92" s="26" t="str">
         <f t="shared" si="2"/>
         <v>x55</v>
       </c>
@@ -2823,59 +2864,59 @@
         <v>7</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93">
         <f t="shared" si="3"/>
         <v>86</v>
       </c>
-      <c r="B93" s="27" t="str">
+      <c r="B93" s="26" t="str">
         <f t="shared" si="2"/>
         <v>x56</v>
       </c>
-      <c r="C93" s="42"/>
-      <c r="D93" s="42"/>
-      <c r="E93" s="42"/>
-      <c r="F93" s="43"/>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C93" s="39"/>
+      <c r="D93" s="39"/>
+      <c r="E93" s="39"/>
+      <c r="F93" s="40"/>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94">
         <f t="shared" si="3"/>
         <v>87</v>
       </c>
-      <c r="B94" s="27" t="str">
+      <c r="B94" s="26" t="str">
         <f t="shared" si="2"/>
         <v>x57</v>
       </c>
-      <c r="C94" s="42"/>
-      <c r="D94" s="42"/>
-      <c r="E94" s="42"/>
-      <c r="F94" s="43"/>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C94" s="39"/>
+      <c r="D94" s="39"/>
+      <c r="E94" s="39"/>
+      <c r="F94" s="40"/>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95">
         <f t="shared" si="3"/>
         <v>88</v>
       </c>
-      <c r="B95" s="27" t="str">
+      <c r="B95" s="26" t="str">
         <f t="shared" si="2"/>
         <v>x58</v>
       </c>
       <c r="C95" s="11" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D95" s="11" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E95" s="11" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96">
         <f t="shared" si="3"/>
         <v>89</v>
       </c>
-      <c r="B96" s="27" t="str">
+      <c r="B96" s="26" t="str">
         <f t="shared" si="2"/>
         <v>x59</v>
       </c>
@@ -2883,38 +2924,50 @@
       <c r="D96" s="11"/>
       <c r="E96" s="11"/>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97">
         <f t="shared" si="3"/>
         <v>90</v>
       </c>
-      <c r="B97" s="27" t="str">
+      <c r="B97" s="26" t="str">
         <f t="shared" si="2"/>
         <v>x5A</v>
       </c>
-      <c r="C97" s="11"/>
-      <c r="D97" s="11"/>
-      <c r="E97" s="11"/>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C97" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="D97" s="11" t="s">
+        <v>211</v>
+      </c>
+      <c r="E97" s="11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98">
         <f t="shared" si="3"/>
         <v>91</v>
       </c>
-      <c r="B98" s="27" t="str">
+      <c r="B98" s="26" t="str">
         <f t="shared" si="2"/>
         <v>x5B</v>
       </c>
-      <c r="C98" s="11"/>
-      <c r="D98" s="11"/>
-      <c r="E98" s="11"/>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C98" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="D98" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="E98" s="11" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99">
         <f t="shared" si="3"/>
         <v>92</v>
       </c>
-      <c r="B99" s="27" t="str">
+      <c r="B99" s="26" t="str">
         <f t="shared" si="2"/>
         <v>x5C</v>
       </c>
@@ -2922,38 +2975,50 @@
       <c r="D99" s="11"/>
       <c r="E99" s="11"/>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100">
         <f t="shared" si="3"/>
         <v>93</v>
       </c>
-      <c r="B100" s="27" t="str">
+      <c r="B100" s="26" t="str">
         <f t="shared" si="2"/>
         <v>x5D</v>
       </c>
-      <c r="C100" s="11"/>
-      <c r="D100" s="11"/>
-      <c r="E100" s="11"/>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C100" s="11" t="s">
+        <v>216</v>
+      </c>
+      <c r="D100" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="E100" s="11" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101">
         <f t="shared" si="3"/>
         <v>94</v>
       </c>
-      <c r="B101" s="27" t="str">
+      <c r="B101" s="26" t="str">
         <f t="shared" si="2"/>
         <v>x5E</v>
       </c>
-      <c r="C101" s="11"/>
-      <c r="D101" s="11"/>
-      <c r="E101" s="11"/>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C101" s="38" t="s">
+        <v>219</v>
+      </c>
+      <c r="D101" s="38" t="s">
+        <v>220</v>
+      </c>
+      <c r="E101" s="11" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102">
         <f t="shared" si="3"/>
         <v>95</v>
       </c>
-      <c r="B102" s="27" t="str">
+      <c r="B102" s="26" t="str">
         <f t="shared" si="2"/>
         <v>x5F</v>
       </c>
@@ -2961,12 +3026,12 @@
       <c r="D102" s="11"/>
       <c r="E102" s="11"/>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103">
         <f t="shared" si="3"/>
         <v>96</v>
       </c>
-      <c r="B103" s="27" t="str">
+      <c r="B103" s="26" t="str">
         <f t="shared" si="2"/>
         <v>x60</v>
       </c>
@@ -2974,12 +3039,12 @@
       <c r="D103" s="11"/>
       <c r="E103" s="11"/>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104">
         <f t="shared" si="3"/>
         <v>97</v>
       </c>
-      <c r="B104" s="27" t="str">
+      <c r="B104" s="26" t="str">
         <f t="shared" si="2"/>
         <v>x61</v>
       </c>
@@ -2987,12 +3052,12 @@
       <c r="D104" s="11"/>
       <c r="E104" s="11"/>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105">
         <f t="shared" si="3"/>
         <v>98</v>
       </c>
-      <c r="B105" s="27" t="str">
+      <c r="B105" s="26" t="str">
         <f t="shared" si="2"/>
         <v>x62</v>
       </c>
@@ -3000,12 +3065,12 @@
       <c r="D105" s="11"/>
       <c r="E105" s="11"/>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106">
         <f t="shared" si="3"/>
         <v>99</v>
       </c>
-      <c r="B106" s="27" t="str">
+      <c r="B106" s="26" t="str">
         <f t="shared" si="2"/>
         <v>x63</v>
       </c>
@@ -3013,12 +3078,12 @@
       <c r="D106" s="11"/>
       <c r="E106" s="11"/>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107">
         <f t="shared" si="3"/>
         <v>100</v>
       </c>
-      <c r="B107" s="27" t="str">
+      <c r="B107" s="26" t="str">
         <f t="shared" si="2"/>
         <v>x64</v>
       </c>
@@ -3026,12 +3091,12 @@
       <c r="D107" s="11"/>
       <c r="E107" s="11"/>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108">
         <f t="shared" si="3"/>
         <v>101</v>
       </c>
-      <c r="B108" s="27" t="str">
+      <c r="B108" s="26" t="str">
         <f t="shared" si="2"/>
         <v>x65</v>
       </c>
@@ -3039,22 +3104,22 @@
       <c r="D108" s="11"/>
       <c r="E108" s="11"/>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109">
         <f t="shared" si="3"/>
         <v>102</v>
       </c>
-      <c r="B109" s="27" t="str">
+      <c r="B109" s="26" t="str">
         <f t="shared" si="2"/>
         <v>x66</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110">
         <f t="shared" si="3"/>
         <v>103</v>
       </c>
-      <c r="B110" s="27" t="str">
+      <c r="B110" s="26" t="str">
         <f t="shared" si="2"/>
         <v>x67</v>
       </c>
@@ -3065,12 +3130,12 @@
         <v>144</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111">
         <f t="shared" si="3"/>
         <v>104</v>
       </c>
-      <c r="B111" s="27" t="str">
+      <c r="B111" s="26" t="str">
         <f t="shared" si="2"/>
         <v>x68</v>
       </c>
@@ -3078,12 +3143,12 @@
         <v>141</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112">
         <f t="shared" si="3"/>
         <v>105</v>
       </c>
-      <c r="B112" s="27" t="str">
+      <c r="B112" s="26" t="str">
         <f t="shared" si="2"/>
         <v>x69</v>
       </c>
@@ -3091,12 +3156,12 @@
         <v>142</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113">
         <f t="shared" si="3"/>
         <v>106</v>
       </c>
-      <c r="B113" s="27" t="str">
+      <c r="B113" s="26" t="str">
         <f t="shared" si="2"/>
         <v>x6A</v>
       </c>
@@ -3104,12 +3169,12 @@
         <v>145</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114">
         <f t="shared" si="3"/>
         <v>107</v>
       </c>
-      <c r="B114" s="27" t="str">
+      <c r="B114" s="26" t="str">
         <f t="shared" si="2"/>
         <v>x6B</v>
       </c>
@@ -3117,34 +3182,34 @@
         <v>146</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115">
         <f t="shared" si="3"/>
         <v>108</v>
       </c>
-      <c r="B115" s="27" t="str">
+      <c r="B115" s="26" t="str">
         <f t="shared" si="2"/>
         <v>x6C</v>
       </c>
-      <c r="C115" s="31" t="s">
+      <c r="C115" s="30" t="s">
         <v>119</v>
       </c>
-      <c r="D115" s="31" t="s">
+      <c r="D115" s="30" t="s">
         <v>121</v>
       </c>
-      <c r="E115" s="31" t="s">
+      <c r="E115" s="30" t="s">
         <v>6</v>
       </c>
       <c r="F115" s="5" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116">
         <f t="shared" si="3"/>
         <v>109</v>
       </c>
-      <c r="B116" s="27" t="str">
+      <c r="B116" s="26" t="str">
         <f t="shared" si="2"/>
         <v>x6D</v>
       </c>
@@ -3161,12 +3226,12 @@
         <v>86</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117">
         <f t="shared" si="3"/>
         <v>110</v>
       </c>
-      <c r="B117" s="27" t="str">
+      <c r="B117" s="26" t="str">
         <f t="shared" si="2"/>
         <v>x6E</v>
       </c>
@@ -3177,15 +3242,15 @@
         <v>127</v>
       </c>
       <c r="F117" s="5" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118">
         <f t="shared" si="3"/>
         <v>111</v>
       </c>
-      <c r="B118" s="27" t="str">
+      <c r="B118" s="26" t="str">
         <f t="shared" si="2"/>
         <v>x6F</v>
       </c>
@@ -3196,12 +3261,12 @@
         <v>125</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119">
         <f t="shared" si="3"/>
         <v>112</v>
       </c>
-      <c r="B119" s="27" t="str">
+      <c r="B119" s="26" t="str">
         <f t="shared" si="2"/>
         <v>x70</v>
       </c>
@@ -3212,28 +3277,28 @@
         <v>126</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120">
         <f t="shared" si="3"/>
         <v>113</v>
       </c>
-      <c r="B120" s="27" t="str">
+      <c r="B120" s="26" t="str">
         <f t="shared" si="2"/>
         <v>x71</v>
       </c>
       <c r="C120" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="D120" s="32" t="s">
+      <c r="D120" s="31" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121">
         <f t="shared" si="3"/>
         <v>114</v>
       </c>
-      <c r="B121" s="27" t="str">
+      <c r="B121" s="26" t="str">
         <f t="shared" si="2"/>
         <v>x72</v>
       </c>
@@ -3244,44 +3309,44 @@
         <v>135</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122">
         <f t="shared" si="3"/>
         <v>115</v>
       </c>
-      <c r="B122" s="27" t="str">
+      <c r="B122" s="26" t="str">
         <f t="shared" si="2"/>
         <v>x73</v>
       </c>
       <c r="C122" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="D122" s="32" t="s">
+      <c r="D122" s="31" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123">
         <f t="shared" si="3"/>
         <v>116</v>
       </c>
-      <c r="B123" s="27" t="str">
+      <c r="B123" s="26" t="str">
         <f t="shared" si="2"/>
         <v>x74</v>
       </c>
       <c r="C123" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="D123" s="32" t="s">
+      <c r="D123" s="31" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124">
         <f t="shared" si="3"/>
         <v>117</v>
       </c>
-      <c r="B124" s="27" t="str">
+      <c r="B124" s="26" t="str">
         <f t="shared" si="2"/>
         <v>x75</v>
       </c>
@@ -3292,44 +3357,44 @@
         <v>137</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125">
         <f t="shared" si="3"/>
         <v>118</v>
       </c>
-      <c r="B125" s="27" t="str">
+      <c r="B125" s="26" t="str">
         <f t="shared" si="2"/>
         <v>x76</v>
       </c>
       <c r="C125" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="D125" s="32" t="s">
+      <c r="D125" s="31" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126">
         <f t="shared" si="3"/>
         <v>119</v>
       </c>
-      <c r="B126" s="27" t="str">
+      <c r="B126" s="26" t="str">
         <f t="shared" si="2"/>
         <v>x77</v>
       </c>
       <c r="C126" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="D126" s="32" t="s">
+      <c r="D126" s="31" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127">
         <f t="shared" si="3"/>
         <v>120</v>
       </c>
-      <c r="B127" s="27" t="str">
+      <c r="B127" s="26" t="str">
         <f t="shared" si="2"/>
         <v>x78</v>
       </c>
@@ -3337,12 +3402,12 @@
         <v>147</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128">
         <f t="shared" si="3"/>
         <v>121</v>
       </c>
-      <c r="B128" s="27" t="str">
+      <c r="B128" s="26" t="str">
         <f t="shared" si="2"/>
         <v>x79</v>
       </c>
@@ -3353,56 +3418,56 @@
         <v>143</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129">
         <f t="shared" si="3"/>
         <v>122</v>
       </c>
-      <c r="B129" s="27" t="str">
+      <c r="B129" s="26" t="str">
         <f t="shared" si="2"/>
         <v>x7A</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130">
         <f t="shared" si="3"/>
         <v>123</v>
       </c>
-      <c r="B130" s="27" t="str">
+      <c r="B130" s="26" t="str">
         <f t="shared" si="2"/>
         <v>x7B</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131">
         <f t="shared" si="3"/>
         <v>124</v>
       </c>
-      <c r="B131" s="27" t="str">
+      <c r="B131" s="26" t="str">
         <f t="shared" si="2"/>
         <v>x7C</v>
       </c>
-      <c r="C131" s="36"/>
-      <c r="D131" s="36"/>
-      <c r="E131" s="36"/>
-      <c r="F131" s="37"/>
-    </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C131" s="35"/>
+      <c r="D131" s="35"/>
+      <c r="E131" s="35"/>
+      <c r="F131" s="36"/>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132">
         <f t="shared" si="3"/>
         <v>125</v>
       </c>
-      <c r="B132" s="27" t="str">
+      <c r="B132" s="26" t="str">
         <f t="shared" si="2"/>
         <v>x7D</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133">
         <f t="shared" si="3"/>
         <v>126</v>
       </c>
-      <c r="B133" s="27" t="str">
+      <c r="B133" s="26" t="str">
         <f t="shared" si="2"/>
         <v>x7E</v>
       </c>
@@ -3416,12 +3481,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A134">
         <f t="shared" si="3"/>
         <v>127</v>
       </c>
-      <c r="B134" s="27" t="str">
+      <c r="B134" s="26" t="str">
         <f t="shared" si="2"/>
         <v>x7F</v>
       </c>
@@ -3435,491 +3500,491 @@
         <v>7</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>128</v>
       </c>
-      <c r="B135" s="27" t="str">
+      <c r="B135" s="26" t="str">
         <f t="shared" si="2"/>
         <v>x80</v>
       </c>
       <c r="C135" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D135" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E135" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136">
         <f>A135+1</f>
         <v>129</v>
       </c>
-      <c r="B136" s="27" t="str">
+      <c r="B136" s="26" t="str">
         <f t="shared" ref="B136:B175" si="4">"x" &amp; DEC2HEX(A136,2)</f>
         <v>x81</v>
       </c>
-      <c r="C136" s="38" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A137" s="38">
+      <c r="C136" s="37" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A137" s="37">
         <f t="shared" ref="A137:A175" si="5">A136+1</f>
         <v>130</v>
       </c>
-      <c r="B137" s="27" t="str">
+      <c r="B137" s="26" t="str">
         <f t="shared" si="4"/>
         <v>x82</v>
       </c>
-      <c r="C137" s="38" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A138" s="38">
+      <c r="C137" s="37" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A138" s="37">
         <f t="shared" si="5"/>
         <v>131</v>
       </c>
-      <c r="B138" s="27" t="str">
+      <c r="B138" s="26" t="str">
         <f t="shared" si="4"/>
         <v>x83</v>
       </c>
-      <c r="C138" s="38" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A139" s="38">
+      <c r="C138" s="37" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A139" s="37">
         <f t="shared" si="5"/>
         <v>132</v>
       </c>
-      <c r="B139" s="27" t="str">
+      <c r="B139" s="26" t="str">
         <f t="shared" si="4"/>
         <v>x84</v>
       </c>
-      <c r="C139" s="38" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A140" s="38">
+      <c r="C139" s="37" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A140" s="37">
         <f t="shared" si="5"/>
         <v>133</v>
       </c>
-      <c r="B140" s="27" t="str">
+      <c r="B140" s="26" t="str">
         <f t="shared" si="4"/>
         <v>x85</v>
       </c>
-      <c r="C140" s="38" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A141" s="38">
+      <c r="C140" s="37" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A141" s="37">
         <f t="shared" si="5"/>
         <v>134</v>
       </c>
-      <c r="B141" s="27" t="str">
+      <c r="B141" s="26" t="str">
         <f t="shared" si="4"/>
         <v>x86</v>
       </c>
-      <c r="C141" s="38" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A142" s="38">
+      <c r="C141" s="37" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A142" s="37">
         <f t="shared" si="5"/>
         <v>135</v>
       </c>
-      <c r="B142" s="27" t="str">
+      <c r="B142" s="26" t="str">
         <f t="shared" si="4"/>
         <v>x87</v>
       </c>
-      <c r="C142" s="38" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A143" s="38">
+      <c r="C142" s="37" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A143" s="37">
         <f t="shared" si="5"/>
         <v>136</v>
       </c>
-      <c r="B143" s="27" t="str">
+      <c r="B143" s="26" t="str">
         <f t="shared" si="4"/>
         <v>x88</v>
       </c>
-      <c r="C143" s="38" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A144" s="38">
+      <c r="C143" s="37" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A144" s="37">
         <f t="shared" si="5"/>
         <v>137</v>
       </c>
-      <c r="B144" s="27" t="str">
+      <c r="B144" s="26" t="str">
         <f t="shared" si="4"/>
         <v>x89</v>
       </c>
-      <c r="C144" s="38" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A145" s="38">
+      <c r="C144" s="37" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A145" s="37">
         <f t="shared" si="5"/>
         <v>138</v>
       </c>
-      <c r="B145" s="27" t="str">
+      <c r="B145" s="26" t="str">
         <f t="shared" si="4"/>
         <v>x8A</v>
       </c>
-      <c r="C145" s="38" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A146" s="38">
+      <c r="C145" s="37" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A146" s="37">
         <f t="shared" si="5"/>
         <v>139</v>
       </c>
-      <c r="B146" s="27" t="str">
+      <c r="B146" s="26" t="str">
         <f t="shared" si="4"/>
         <v>x8B</v>
       </c>
-      <c r="C146" s="38" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A147" s="38">
+      <c r="C146" s="37" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A147" s="37">
         <f t="shared" si="5"/>
         <v>140</v>
       </c>
-      <c r="B147" s="27" t="str">
+      <c r="B147" s="26" t="str">
         <f t="shared" si="4"/>
         <v>x8C</v>
       </c>
-      <c r="C147" s="38" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A148" s="38">
+      <c r="C147" s="37" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A148" s="37">
         <f t="shared" si="5"/>
         <v>141</v>
       </c>
-      <c r="B148" s="27" t="str">
+      <c r="B148" s="26" t="str">
         <f t="shared" si="4"/>
         <v>x8D</v>
       </c>
-      <c r="C148" s="38" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A149" s="38">
+      <c r="C148" s="37" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A149" s="37">
         <f t="shared" si="5"/>
         <v>142</v>
       </c>
-      <c r="B149" s="27" t="str">
+      <c r="B149" s="26" t="str">
         <f t="shared" si="4"/>
         <v>x8E</v>
       </c>
-      <c r="C149" s="38" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A150" s="38">
+      <c r="C149" s="37" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A150" s="37">
         <f t="shared" si="5"/>
         <v>143</v>
       </c>
-      <c r="B150" s="27" t="str">
+      <c r="B150" s="26" t="str">
         <f t="shared" si="4"/>
         <v>x8F</v>
       </c>
-      <c r="C150" s="38" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A151" s="38">
+      <c r="C150" s="37" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A151" s="37">
         <f t="shared" si="5"/>
         <v>144</v>
       </c>
-      <c r="B151" s="27" t="str">
+      <c r="B151" s="26" t="str">
         <f t="shared" si="4"/>
         <v>x90</v>
       </c>
-      <c r="C151" s="38" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A152" s="38">
+      <c r="C151" s="37" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A152" s="37">
         <f t="shared" si="5"/>
         <v>145</v>
       </c>
-      <c r="B152" s="27" t="str">
+      <c r="B152" s="26" t="str">
         <f t="shared" si="4"/>
         <v>x91</v>
       </c>
-      <c r="C152" s="38" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A153" s="38">
+      <c r="C152" s="37" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A153" s="37">
         <f t="shared" si="5"/>
         <v>146</v>
       </c>
-      <c r="B153" s="27" t="str">
+      <c r="B153" s="26" t="str">
         <f t="shared" si="4"/>
         <v>x92</v>
       </c>
-      <c r="C153" s="38" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A154" s="38">
+      <c r="C153" s="37" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A154" s="37">
         <f t="shared" si="5"/>
         <v>147</v>
       </c>
-      <c r="B154" s="27" t="str">
+      <c r="B154" s="26" t="str">
         <f t="shared" si="4"/>
         <v>x93</v>
       </c>
-      <c r="C154" s="38" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A155" s="38">
+      <c r="C154" s="37" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A155" s="37">
         <f t="shared" si="5"/>
         <v>148</v>
       </c>
-      <c r="B155" s="27" t="str">
+      <c r="B155" s="26" t="str">
         <f t="shared" si="4"/>
         <v>x94</v>
       </c>
-      <c r="C155" s="38" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A156" s="38">
+      <c r="C155" s="37" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A156" s="37">
         <f t="shared" si="5"/>
         <v>149</v>
       </c>
-      <c r="B156" s="27" t="str">
+      <c r="B156" s="26" t="str">
         <f t="shared" si="4"/>
         <v>x95</v>
       </c>
-      <c r="C156" s="38" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A157" s="38">
+      <c r="C156" s="37" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A157" s="37">
         <f t="shared" si="5"/>
         <v>150</v>
       </c>
-      <c r="B157" s="27" t="str">
+      <c r="B157" s="26" t="str">
         <f t="shared" si="4"/>
         <v>x96</v>
       </c>
-      <c r="C157" s="38" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A158" s="38">
+      <c r="C157" s="37" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A158" s="37">
         <f t="shared" si="5"/>
         <v>151</v>
       </c>
-      <c r="B158" s="27" t="str">
+      <c r="B158" s="26" t="str">
         <f t="shared" si="4"/>
         <v>x97</v>
       </c>
-      <c r="C158" s="38" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A159" s="38">
+      <c r="C158" s="37" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A159" s="37">
         <f t="shared" si="5"/>
         <v>152</v>
       </c>
-      <c r="B159" s="27" t="str">
+      <c r="B159" s="26" t="str">
         <f t="shared" si="4"/>
         <v>x98</v>
       </c>
-      <c r="C159" s="38"/>
-    </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A160" s="38">
+      <c r="C159" s="37"/>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A160" s="37">
         <f t="shared" si="5"/>
         <v>153</v>
       </c>
-      <c r="B160" s="27" t="str">
+      <c r="B160" s="26" t="str">
         <f t="shared" si="4"/>
         <v>x99</v>
       </c>
-      <c r="C160" s="38"/>
-    </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A161" s="38">
+      <c r="C160" s="37"/>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A161" s="37">
         <f t="shared" si="5"/>
         <v>154</v>
       </c>
-      <c r="B161" s="27" t="str">
+      <c r="B161" s="26" t="str">
         <f t="shared" si="4"/>
         <v>x9A</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A162" s="38">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A162" s="37">
         <f t="shared" si="5"/>
         <v>155</v>
       </c>
-      <c r="B162" s="27" t="str">
+      <c r="B162" s="26" t="str">
         <f t="shared" si="4"/>
         <v>x9B</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A163" s="38">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A163" s="37">
         <f t="shared" si="5"/>
         <v>156</v>
       </c>
-      <c r="B163" s="27" t="str">
+      <c r="B163" s="26" t="str">
         <f t="shared" si="4"/>
         <v>x9C</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A164" s="38">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A164" s="37">
         <f t="shared" si="5"/>
         <v>157</v>
       </c>
-      <c r="B164" s="27" t="str">
+      <c r="B164" s="26" t="str">
         <f t="shared" si="4"/>
         <v>x9D</v>
       </c>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A165" s="38">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A165" s="37">
         <f t="shared" si="5"/>
         <v>158</v>
       </c>
-      <c r="B165" s="27" t="str">
+      <c r="B165" s="26" t="str">
         <f t="shared" si="4"/>
         <v>x9E</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A166" s="38">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A166" s="37">
         <f t="shared" si="5"/>
         <v>159</v>
       </c>
-      <c r="B166" s="27" t="str">
+      <c r="B166" s="26" t="str">
         <f t="shared" si="4"/>
         <v>x9F</v>
       </c>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A167" s="38">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A167" s="37">
         <f t="shared" si="5"/>
         <v>160</v>
       </c>
-      <c r="B167" s="27" t="str">
+      <c r="B167" s="26" t="str">
         <f t="shared" si="4"/>
         <v>xA0</v>
       </c>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A168" s="38">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A168" s="37">
         <f t="shared" si="5"/>
         <v>161</v>
       </c>
-      <c r="B168" s="27" t="str">
+      <c r="B168" s="26" t="str">
         <f t="shared" si="4"/>
         <v>xA1</v>
       </c>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A169" s="38">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A169" s="37">
         <f t="shared" si="5"/>
         <v>162</v>
       </c>
-      <c r="B169" s="27" t="str">
+      <c r="B169" s="26" t="str">
         <f t="shared" si="4"/>
         <v>xA2</v>
       </c>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A170" s="38">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A170" s="37">
         <f t="shared" si="5"/>
         <v>163</v>
       </c>
-      <c r="B170" s="27" t="str">
+      <c r="B170" s="26" t="str">
         <f t="shared" si="4"/>
         <v>xA3</v>
       </c>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A171" s="38">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A171" s="37">
         <f t="shared" si="5"/>
         <v>164</v>
       </c>
-      <c r="B171" s="27" t="str">
+      <c r="B171" s="26" t="str">
         <f t="shared" si="4"/>
         <v>xA4</v>
       </c>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A172" s="38">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A172" s="37">
         <f t="shared" si="5"/>
         <v>165</v>
       </c>
-      <c r="B172" s="27" t="str">
+      <c r="B172" s="26" t="str">
         <f t="shared" si="4"/>
         <v>xA5</v>
       </c>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A173" s="38">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A173" s="37">
         <f t="shared" si="5"/>
         <v>166</v>
       </c>
-      <c r="B173" s="27" t="str">
+      <c r="B173" s="26" t="str">
         <f t="shared" si="4"/>
         <v>xA6</v>
       </c>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A174" s="38">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A174" s="37">
         <f t="shared" si="5"/>
         <v>167</v>
       </c>
-      <c r="B174" s="27" t="str">
+      <c r="B174" s="26" t="str">
         <f t="shared" si="4"/>
         <v>xA7</v>
       </c>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A175" s="38">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A175" s="37">
         <f t="shared" si="5"/>
         <v>168</v>
       </c>
-      <c r="B175" s="27" t="str">
+      <c r="B175" s="26" t="str">
         <f t="shared" si="4"/>
         <v>xA8</v>
       </c>

</xml_diff>

<commit_message>
Working FIR low pass. V0.12
</commit_message>
<xml_diff>
--- a/doc/firmware-register-map.xlsx
+++ b/doc/firmware-register-map.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="223">
   <si>
     <t>Register Map</t>
   </si>
@@ -665,15 +665,6 @@
     <t>x0000FF</t>
   </si>
   <si>
-    <t>low pass filter register (2)</t>
-  </si>
-  <si>
-    <t>x000005</t>
-  </si>
-  <si>
-    <t>lower 8 bits = post filter bitshift (division)</t>
-  </si>
-  <si>
     <t>dynamic beam mask register</t>
   </si>
   <si>
@@ -699,6 +690,9 @@
   </si>
   <si>
     <t>dynamic beam mask value</t>
+  </si>
+  <si>
+    <t>x000001</t>
   </si>
 </sst>
 </file>
@@ -1204,8 +1198,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="B76" workbookViewId="0">
+      <selection activeCell="E98" sqref="E98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1746,7 +1740,7 @@
         <v>x17</v>
       </c>
       <c r="C30" s="22" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="D30" s="22" t="s">
         <v>61</v>
@@ -1755,7 +1749,7 @@
         <v>6</v>
       </c>
       <c r="F30" s="19" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1928,7 +1922,7 @@
         <v>x22</v>
       </c>
       <c r="C41" s="21" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="D41" s="38" t="s">
         <v>15</v>
@@ -1937,7 +1931,7 @@
         <v>6</v>
       </c>
       <c r="F41" s="19" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -2940,7 +2934,7 @@
         <v>211</v>
       </c>
       <c r="E97" s="11" t="s">
-        <v>7</v>
+        <v>222</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
@@ -2952,15 +2946,9 @@
         <f t="shared" si="2"/>
         <v>x5B</v>
       </c>
-      <c r="C98" s="11" t="s">
-        <v>213</v>
-      </c>
-      <c r="D98" s="11" t="s">
-        <v>215</v>
-      </c>
-      <c r="E98" s="11" t="s">
-        <v>214</v>
-      </c>
+      <c r="C98" s="11"/>
+      <c r="D98" s="11"/>
+      <c r="E98" s="11"/>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99">
@@ -2985,13 +2973,13 @@
         <v>x5D</v>
       </c>
       <c r="C100" s="11" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D100" s="11" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="E100" s="11" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
@@ -3004,13 +2992,13 @@
         <v>x5E</v>
       </c>
       <c r="C101" s="38" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="D101" s="38" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="E101" s="11" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fix errors in metadata and beamforming (had redundant beams)
</commit_message>
<xml_diff>
--- a/doc/firmware-register-map.xlsx
+++ b/doc/firmware-register-map.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="225">
   <si>
     <t>Register Map</t>
   </si>
@@ -335,9 +335,6 @@
     <t>default: phased trigger disabled at startup (LSB)</t>
   </si>
   <si>
-    <t>deadtime counter (num 25 MHz clk cycles) refreshed every second</t>
-  </si>
-  <si>
     <t>rdout-&gt;clear  buffer full, set buffer num to zero</t>
   </si>
   <si>
@@ -506,9 +503,6 @@
     <t>update register by writing LSB in reg 40</t>
   </si>
   <si>
-    <t>bit 23 : gate flag ; bits 22-15 : channel mask ; bits 14-0 : beam mask</t>
-  </si>
-  <si>
     <t>x000C03</t>
   </si>
   <si>
@@ -693,6 +687,18 @@
   </si>
   <si>
     <t>x000001</t>
+  </si>
+  <si>
+    <t>deadtime counter (num 31.25 MHz clk cycles) refreshed every second</t>
+  </si>
+  <si>
+    <t>bit 23 : gate flag ; bits 22-15 : channel mask ; bits 14-0 : zeros</t>
+  </si>
+  <si>
+    <t>metadata-&gt; user beam mask</t>
+  </si>
+  <si>
+    <t>24 bit user beam mask (register 80 value)</t>
   </si>
 </sst>
 </file>
@@ -841,7 +847,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -916,6 +922,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1198,8 +1207,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B76" workbookViewId="0">
-      <selection activeCell="E98" sqref="E98"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1215,7 +1224,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="41" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B1" s="41"/>
       <c r="C1" s="41"/>
@@ -1248,7 +1257,7 @@
       <c r="B4" s="43"/>
       <c r="C4" s="1"/>
       <c r="D4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>27</v>
@@ -1342,7 +1351,7 @@
         <v>15</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1393,13 +1402,13 @@
         <v>x06</v>
       </c>
       <c r="C13" t="s">
+        <v>115</v>
+      </c>
+      <c r="D13" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="F13" s="5" t="s">
         <v>117</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1597,7 +1606,7 @@
         <v>6</v>
       </c>
       <c r="F23" s="19" t="s">
-        <v>103</v>
+        <v>221</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1610,7 +1619,7 @@
         <v>x11</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D24" s="18" t="s">
         <v>61</v>
@@ -1619,7 +1628,7 @@
         <v>6</v>
       </c>
       <c r="F24" s="19" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1641,7 +1650,7 @@
         <v>6</v>
       </c>
       <c r="F25" s="19" t="s">
-        <v>160</v>
+        <v>222</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1674,7 +1683,7 @@
         <v>x14</v>
       </c>
       <c r="C27" s="22" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D27" s="18" t="s">
         <v>61</v>
@@ -1683,7 +1692,7 @@
         <v>6</v>
       </c>
       <c r="F27" s="19" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1696,7 +1705,7 @@
         <v>x15</v>
       </c>
       <c r="C28" s="22" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D28" s="18" t="s">
         <v>61</v>
@@ -1705,7 +1714,7 @@
         <v>6</v>
       </c>
       <c r="F28" s="19" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -1718,7 +1727,7 @@
         <v>x16</v>
       </c>
       <c r="C29" s="22" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D29" s="22" t="s">
         <v>61</v>
@@ -1727,7 +1736,7 @@
         <v>6</v>
       </c>
       <c r="F29" s="19" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -1740,7 +1749,7 @@
         <v>x17</v>
       </c>
       <c r="C30" s="22" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D30" s="22" t="s">
         <v>61</v>
@@ -1749,7 +1758,7 @@
         <v>6</v>
       </c>
       <c r="F30" s="19" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1761,12 +1770,18 @@
         <f t="shared" si="0"/>
         <v>x18</v>
       </c>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18"/>
+      <c r="C31" s="22" t="s">
+        <v>223</v>
+      </c>
+      <c r="D31" s="22" t="s">
+        <v>61</v>
+      </c>
       <c r="E31" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="F31" s="19"/>
+      <c r="F31" s="19" t="s">
+        <v>224</v>
+      </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="17">
@@ -1922,16 +1937,16 @@
         <v>x22</v>
       </c>
       <c r="C41" s="21" t="s">
-        <v>221</v>
-      </c>
-      <c r="D41" s="38" t="s">
+        <v>219</v>
+      </c>
+      <c r="D41" s="21" t="s">
         <v>15</v>
       </c>
       <c r="E41" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="F41" s="19" t="s">
-        <v>220</v>
+      <c r="F41" s="44" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -2042,10 +2057,10 @@
         <v>x28</v>
       </c>
       <c r="C47" t="s">
+        <v>153</v>
+      </c>
+      <c r="D47" t="s">
         <v>154</v>
-      </c>
-      <c r="D47" t="s">
-        <v>155</v>
       </c>
       <c r="E47" t="s">
         <v>6</v>
@@ -2064,13 +2079,13 @@
         <v>58</v>
       </c>
       <c r="D48" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E48" t="s">
         <v>6</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -2115,13 +2130,13 @@
         <v>x2C</v>
       </c>
       <c r="C51" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D51" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -2134,13 +2149,13 @@
         <v>x2D</v>
       </c>
       <c r="C52" s="32" t="s">
+        <v>156</v>
+      </c>
+      <c r="D52" s="32" t="s">
+        <v>158</v>
+      </c>
+      <c r="F52" s="5" t="s">
         <v>157</v>
-      </c>
-      <c r="D52" s="32" t="s">
-        <v>159</v>
-      </c>
-      <c r="F52" s="5" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -2182,7 +2197,7 @@
         <v>57</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -2214,7 +2229,7 @@
         <v>6</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -2236,7 +2251,7 @@
         <v>6</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -2258,7 +2273,7 @@
         <v>6</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
@@ -2322,7 +2337,7 @@
         <v>28</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E63" s="3" t="s">
         <v>6</v>
@@ -2341,7 +2356,7 @@
         <v>29</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E64" s="3" t="s">
         <v>6</v>
@@ -2360,7 +2375,7 @@
         <v>30</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E65" s="3" t="s">
         <v>6</v>
@@ -2379,7 +2394,7 @@
         <v>31</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E66" s="3" t="s">
         <v>6</v>
@@ -2632,16 +2647,16 @@
         <v>x4B</v>
       </c>
       <c r="C82" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="D82" s="24" t="s">
+        <v>151</v>
+      </c>
+      <c r="E82" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="F82" s="33" t="s">
         <v>150</v>
-      </c>
-      <c r="D82" s="24" t="s">
-        <v>152</v>
-      </c>
-      <c r="E82" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="F82" s="33" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="83" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2657,13 +2672,13 @@
         <v>50</v>
       </c>
       <c r="D83" s="5" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E83" t="s">
+        <v>113</v>
+      </c>
+      <c r="F83" s="5" t="s">
         <v>114</v>
-      </c>
-      <c r="F83" s="5" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
@@ -2676,16 +2691,16 @@
         <v>x4D</v>
       </c>
       <c r="C84" t="s">
+        <v>103</v>
+      </c>
+      <c r="D84" t="s">
         <v>104</v>
-      </c>
-      <c r="D84" t="s">
-        <v>105</v>
       </c>
       <c r="E84" t="s">
         <v>7</v>
       </c>
       <c r="F84" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
@@ -2720,10 +2735,10 @@
         <v>x4F</v>
       </c>
       <c r="C86" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D86" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E86" t="s">
         <v>7</v>
@@ -2764,13 +2779,13 @@
         <v>74</v>
       </c>
       <c r="D88" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E88" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="F88" s="5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
@@ -2783,13 +2798,13 @@
         <v>x52</v>
       </c>
       <c r="C89" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D89" s="5" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E89" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="F89" s="5" t="s">
         <v>102</v>
@@ -2808,13 +2823,13 @@
         <v>98</v>
       </c>
       <c r="D90" s="5" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E90" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F90" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="91" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2827,16 +2842,16 @@
         <v>x54</v>
       </c>
       <c r="C91" t="s">
+        <v>107</v>
+      </c>
+      <c r="D91" t="s">
         <v>108</v>
-      </c>
-      <c r="D91" t="s">
-        <v>109</v>
       </c>
       <c r="E91" t="s">
         <v>7</v>
       </c>
       <c r="F91" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="92" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2849,10 +2864,10 @@
         <v>x55</v>
       </c>
       <c r="C92" t="s">
+        <v>122</v>
+      </c>
+      <c r="D92" s="5" t="s">
         <v>123</v>
-      </c>
-      <c r="D92" s="5" t="s">
-        <v>124</v>
       </c>
       <c r="E92" s="11" t="s">
         <v>7</v>
@@ -2896,10 +2911,10 @@
         <v>x58</v>
       </c>
       <c r="C95" s="11" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D95" s="11" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E95" s="11" t="s">
         <v>7</v>
@@ -2928,13 +2943,13 @@
         <v>x5A</v>
       </c>
       <c r="C97" s="11" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D97" s="11" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E97" s="11" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
@@ -2973,13 +2988,13 @@
         <v>x5D</v>
       </c>
       <c r="C100" s="11" t="s">
+        <v>211</v>
+      </c>
+      <c r="D100" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="E100" s="11" t="s">
         <v>213</v>
-      </c>
-      <c r="D100" s="11" t="s">
-        <v>214</v>
-      </c>
-      <c r="E100" s="11" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
@@ -2992,13 +3007,13 @@
         <v>x5E</v>
       </c>
       <c r="C101" s="38" t="s">
+        <v>214</v>
+      </c>
+      <c r="D101" s="38" t="s">
+        <v>215</v>
+      </c>
+      <c r="E101" s="11" t="s">
         <v>216</v>
-      </c>
-      <c r="D101" s="38" t="s">
-        <v>217</v>
-      </c>
-      <c r="E101" s="11" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
@@ -3112,10 +3127,10 @@
         <v>x67</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D110" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
@@ -3128,7 +3143,7 @@
         <v>x68</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
@@ -3141,7 +3156,7 @@
         <v>x69</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
@@ -3154,7 +3169,7 @@
         <v>x6A</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
@@ -3167,7 +3182,7 @@
         <v>x6B</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
@@ -3180,16 +3195,16 @@
         <v>x6C</v>
       </c>
       <c r="C115" s="30" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D115" s="30" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E115" s="30" t="s">
         <v>6</v>
       </c>
       <c r="F115" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
@@ -3224,13 +3239,13 @@
         <v>x6E</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D117" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F117" s="5" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
@@ -3243,10 +3258,10 @@
         <v>x6F</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D118" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
@@ -3259,10 +3274,10 @@
         <v>x70</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D119" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
@@ -3275,10 +3290,10 @@
         <v>x71</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D120" s="31" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
@@ -3291,10 +3306,10 @@
         <v>x72</v>
       </c>
       <c r="C121" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D121" t="s">
         <v>134</v>
-      </c>
-      <c r="D121" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
@@ -3307,10 +3322,10 @@
         <v>x73</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D122" s="31" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
@@ -3323,10 +3338,10 @@
         <v>x74</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D123" s="31" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
@@ -3339,10 +3354,10 @@
         <v>x75</v>
       </c>
       <c r="C124" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="D124" t="s">
         <v>136</v>
-      </c>
-      <c r="D124" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
@@ -3355,10 +3370,10 @@
         <v>x76</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D125" s="31" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
@@ -3371,10 +3386,10 @@
         <v>x77</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D126" s="31" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
@@ -3387,7 +3402,7 @@
         <v>x78</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
@@ -3400,10 +3415,10 @@
         <v>x79</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D128" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
@@ -3497,10 +3512,10 @@
         <v>x80</v>
       </c>
       <c r="C135" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D135" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E135" t="s">
         <v>44</v>
@@ -3516,7 +3531,7 @@
         <v>x81</v>
       </c>
       <c r="C136" s="37" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
@@ -3529,7 +3544,7 @@
         <v>x82</v>
       </c>
       <c r="C137" s="37" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">
@@ -3542,7 +3557,7 @@
         <v>x83</v>
       </c>
       <c r="C138" s="37" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
@@ -3555,7 +3570,7 @@
         <v>x84</v>
       </c>
       <c r="C139" s="37" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.25">
@@ -3568,7 +3583,7 @@
         <v>x85</v>
       </c>
       <c r="C140" s="37" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">
@@ -3581,7 +3596,7 @@
         <v>x86</v>
       </c>
       <c r="C141" s="37" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.25">
@@ -3594,7 +3609,7 @@
         <v>x87</v>
       </c>
       <c r="C142" s="37" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.25">
@@ -3607,7 +3622,7 @@
         <v>x88</v>
       </c>
       <c r="C143" s="37" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
@@ -3620,7 +3635,7 @@
         <v>x89</v>
       </c>
       <c r="C144" s="37" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
@@ -3633,7 +3648,7 @@
         <v>x8A</v>
       </c>
       <c r="C145" s="37" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
@@ -3646,7 +3661,7 @@
         <v>x8B</v>
       </c>
       <c r="C146" s="37" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
@@ -3659,7 +3674,7 @@
         <v>x8C</v>
       </c>
       <c r="C147" s="37" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
@@ -3672,7 +3687,7 @@
         <v>x8D</v>
       </c>
       <c r="C148" s="37" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
@@ -3685,7 +3700,7 @@
         <v>x8E</v>
       </c>
       <c r="C149" s="37" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
@@ -3698,7 +3713,7 @@
         <v>x8F</v>
       </c>
       <c r="C150" s="37" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
@@ -3711,7 +3726,7 @@
         <v>x90</v>
       </c>
       <c r="C151" s="37" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
@@ -3724,7 +3739,7 @@
         <v>x91</v>
       </c>
       <c r="C152" s="37" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
@@ -3737,7 +3752,7 @@
         <v>x92</v>
       </c>
       <c r="C153" s="37" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
@@ -3750,7 +3765,7 @@
         <v>x93</v>
       </c>
       <c r="C154" s="37" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
@@ -3763,7 +3778,7 @@
         <v>x94</v>
       </c>
       <c r="C155" s="37" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
@@ -3776,7 +3791,7 @@
         <v>x95</v>
       </c>
       <c r="C156" s="37" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
@@ -3789,7 +3804,7 @@
         <v>x96</v>
       </c>
       <c r="C157" s="37" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
@@ -3802,7 +3817,7 @@
         <v>x97</v>
       </c>
       <c r="C158" s="37" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
been awhile, some big updates: 1) fix 2d beamforming and 2) add some data-driven trigger vetos
</commit_message>
<xml_diff>
--- a/doc/firmware-register-map.xlsx
+++ b/doc/firmware-register-map.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="234">
   <si>
     <t>Register Map</t>
   </si>
@@ -686,9 +686,6 @@
     <t>dynamic beam mask value</t>
   </si>
   <si>
-    <t>x000001</t>
-  </si>
-  <si>
     <t>deadtime counter (num 31.25 MHz clk cycles) refreshed every second</t>
   </si>
   <si>
@@ -699,6 +696,36 @@
   </si>
   <si>
     <t>24 bit user beam mask (register 80 value)</t>
+  </si>
+  <si>
+    <t>trigger vetos</t>
+  </si>
+  <si>
+    <t>metadata-&gt; veto deadtime counter</t>
+  </si>
+  <si>
+    <t>24 bit veto-induced deadtime per second, counted on 31.25MHz clock</t>
+  </si>
+  <si>
+    <t>saturation trigger veto, cut value</t>
+  </si>
+  <si>
+    <t>lower 8 bits value</t>
+  </si>
+  <si>
+    <t>x00007E</t>
+  </si>
+  <si>
+    <t>126 default value</t>
+  </si>
+  <si>
+    <t>x004003</t>
+  </si>
+  <si>
+    <t>veto width default ix 0x40 * 1/31.25MHz ~ 2 microsecs</t>
+  </si>
+  <si>
+    <t>LSB-&gt;saturation veto ;  LSB+1-&gt;CW veto via delay+sum ; bit 15 to 8: veto pulse width</t>
   </si>
 </sst>
 </file>
@@ -847,7 +874,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -919,12 +946,13 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1207,8 +1235,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+    <sheetView tabSelected="1" topLeftCell="B84" workbookViewId="0">
+      <selection activeCell="D102" sqref="D102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1223,38 +1251,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="43" t="s">
         <v>168</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="41"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
       <c r="F3" s="6"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="42">
+      <c r="A4" s="44">
         <v>43305</v>
       </c>
-      <c r="B4" s="43"/>
+      <c r="B4" s="45"/>
       <c r="C4" s="1"/>
       <c r="D4" t="s">
         <v>172</v>
@@ -1606,7 +1634,7 @@
         <v>6</v>
       </c>
       <c r="F23" s="19" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1650,7 +1678,7 @@
         <v>6</v>
       </c>
       <c r="F25" s="19" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1771,7 +1799,7 @@
         <v>x18</v>
       </c>
       <c r="C31" s="22" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D31" s="22" t="s">
         <v>61</v>
@@ -1780,7 +1808,7 @@
         <v>6</v>
       </c>
       <c r="F31" s="19" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -1792,12 +1820,18 @@
         <f t="shared" si="0"/>
         <v>x19</v>
       </c>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
+      <c r="C32" s="22" t="s">
+        <v>225</v>
+      </c>
+      <c r="D32" s="22" t="s">
+        <v>61</v>
+      </c>
       <c r="E32" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="F32" s="19"/>
+      <c r="F32" s="19" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="17">
@@ -1945,7 +1979,7 @@
       <c r="E41" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="F41" s="44" t="s">
+      <c r="F41" s="41" t="s">
         <v>218</v>
       </c>
     </row>
@@ -2933,7 +2967,7 @@
       <c r="D96" s="11"/>
       <c r="E96" s="11"/>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97">
         <f t="shared" si="3"/>
         <v>90</v>
@@ -2949,10 +2983,10 @@
         <v>209</v>
       </c>
       <c r="E97" s="11" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98">
         <f t="shared" si="3"/>
         <v>91</v>
@@ -2965,7 +2999,7 @@
       <c r="D98" s="11"/>
       <c r="E98" s="11"/>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99">
         <f t="shared" si="3"/>
         <v>92</v>
@@ -2978,7 +3012,7 @@
       <c r="D99" s="11"/>
       <c r="E99" s="11"/>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100">
         <f t="shared" si="3"/>
         <v>93</v>
@@ -2997,7 +3031,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101">
         <f t="shared" si="3"/>
         <v>94</v>
@@ -3016,7 +3050,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102">
         <f t="shared" si="3"/>
         <v>95</v>
@@ -3025,11 +3059,20 @@
         <f t="shared" si="2"/>
         <v>x5F</v>
       </c>
-      <c r="C102" s="11"/>
-      <c r="D102" s="11"/>
-      <c r="E102" s="11"/>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C102" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="D102" s="11" t="s">
+        <v>233</v>
+      </c>
+      <c r="E102" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="F102" s="5" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103">
         <f t="shared" si="3"/>
         <v>96</v>
@@ -3038,11 +3081,20 @@
         <f t="shared" si="2"/>
         <v>x60</v>
       </c>
-      <c r="C103" s="11"/>
-      <c r="D103" s="11"/>
-      <c r="E103" s="11"/>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C103" s="42" t="s">
+        <v>227</v>
+      </c>
+      <c r="D103" s="42" t="s">
+        <v>228</v>
+      </c>
+      <c r="E103" s="42" t="s">
+        <v>229</v>
+      </c>
+      <c r="F103" s="5" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104">
         <f t="shared" si="3"/>
         <v>97</v>
@@ -3055,7 +3107,7 @@
       <c r="D104" s="11"/>
       <c r="E104" s="11"/>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105">
         <f t="shared" si="3"/>
         <v>98</v>
@@ -3068,7 +3120,7 @@
       <c r="D105" s="11"/>
       <c r="E105" s="11"/>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106">
         <f t="shared" si="3"/>
         <v>99</v>
@@ -3081,7 +3133,7 @@
       <c r="D106" s="11"/>
       <c r="E106" s="11"/>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107">
         <f t="shared" si="3"/>
         <v>100</v>
@@ -3094,7 +3146,7 @@
       <c r="D107" s="11"/>
       <c r="E107" s="11"/>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108">
         <f t="shared" si="3"/>
         <v>101</v>
@@ -3107,7 +3159,7 @@
       <c r="D108" s="11"/>
       <c r="E108" s="11"/>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109">
         <f t="shared" si="3"/>
         <v>102</v>
@@ -3117,7 +3169,7 @@
         <v>x66</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110">
         <f t="shared" si="3"/>
         <v>103</v>
@@ -3133,7 +3185,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111">
         <f t="shared" si="3"/>
         <v>104</v>
@@ -3146,7 +3198,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112">
         <f t="shared" si="3"/>
         <v>105</v>

</xml_diff>

<commit_message>
add to trigger vetoing, add in trigger beam verification
</commit_message>
<xml_diff>
--- a/doc/firmware-register-map.xlsx
+++ b/doc/firmware-register-map.xlsx
@@ -707,18 +707,6 @@
     <t>24 bit veto-induced deadtime per second, counted on 31.25MHz clock</t>
   </si>
   <si>
-    <t>saturation trigger veto, cut value</t>
-  </si>
-  <si>
-    <t>lower 8 bits value</t>
-  </si>
-  <si>
-    <t>x00007E</t>
-  </si>
-  <si>
-    <t>126 default value</t>
-  </si>
-  <si>
     <t>x004003</t>
   </si>
   <si>
@@ -726,6 +714,18 @@
   </si>
   <si>
     <t>LSB-&gt;saturation veto ;  LSB+1-&gt;CW veto via delay+sum ; bit 15 to 8: veto pulse width</t>
+  </si>
+  <si>
+    <t>veto cut value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lower 8 bits sat cut value ; next 8 bits cw cut value </t>
+  </si>
+  <si>
+    <t>x00327E</t>
+  </si>
+  <si>
+    <t>126 default value sat value,  50 default for cw cut value</t>
   </si>
 </sst>
 </file>
@@ -1236,7 +1236,7 @@
   <dimension ref="A1:G175"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B84" workbookViewId="0">
-      <selection activeCell="D102" sqref="D102"/>
+      <selection activeCell="F103" sqref="F103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3063,13 +3063,13 @@
         <v>224</v>
       </c>
       <c r="D102" s="11" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="E102" s="11" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="F102" s="5" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
@@ -3082,16 +3082,16 @@
         <v>x60</v>
       </c>
       <c r="C103" s="42" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="D103" s="42" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="E103" s="42" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="F103" s="5" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
add extended power veto
</commit_message>
<xml_diff>
--- a/doc/firmware-register-map.xlsx
+++ b/doc/firmware-register-map.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="236">
   <si>
     <t>Register Map</t>
   </si>
@@ -726,6 +726,12 @@
   </si>
   <si>
     <t>126 default value sat value,  50 default for cw cut value</t>
+  </si>
+  <si>
+    <t>veto status</t>
+  </si>
+  <si>
+    <t>lower two bits (signal veto, beam power veto)</t>
   </si>
 </sst>
 </file>
@@ -1235,8 +1241,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B84" workbookViewId="0">
-      <selection activeCell="F103" sqref="F103"/>
+    <sheetView tabSelected="1" topLeftCell="B24" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1954,8 +1960,12 @@
         <f t="shared" si="0"/>
         <v>x21</v>
       </c>
-      <c r="C40" s="18"/>
-      <c r="D40" s="18"/>
+      <c r="C40" s="18" t="s">
+        <v>234</v>
+      </c>
+      <c r="D40" s="18" t="s">
+        <v>235</v>
+      </c>
       <c r="E40" s="18" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
update veto scheme, tick fw version 1.5
</commit_message>
<xml_diff>
--- a/doc/firmware-register-map.xlsx
+++ b/doc/firmware-register-map.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="239">
   <si>
     <t>Register Map</t>
   </si>
@@ -707,9 +707,6 @@
     <t>24 bit veto-induced deadtime per second, counted on 31.25MHz clock</t>
   </si>
   <si>
-    <t>veto width default ix 0x40 * 1/31.25MHz ~ 2 microsecs</t>
-  </si>
-  <si>
     <t>veto cut value</t>
   </si>
   <si>
@@ -722,16 +719,28 @@
     <t>lower two bits (signal veto, beam power veto)</t>
   </si>
   <si>
-    <t>LSB-&gt;saturation veto ;  LSB+1-&gt;CW veto via delay+sum ; LSB + 2-&gt; sideswipe ; bit 15 to 8: veto pulse width</t>
-  </si>
-  <si>
     <t>lower 8 bits sat cut value ; next 8 bits cw cut value ; top 8 bits sideswipe cut value</t>
   </si>
   <si>
-    <t>x14327E</t>
-  </si>
-  <si>
-    <t>x003000</t>
+    <t>veto width default ix 0x30 * 1/31.25MHz ~ 1.5 microsecs</t>
+  </si>
+  <si>
+    <t>veto cut values 2</t>
+  </si>
+  <si>
+    <t>lower 8 bits extended above threshold (vpp) value</t>
+  </si>
+  <si>
+    <t>x00300F</t>
+  </si>
+  <si>
+    <t>LSB-&gt;saturation veto ;  LSB+1-&gt;CW veto via delay+sum ; LSB + 2-&gt; sideswipe ; LSB + 3-&gt;extended above threshold (regx61) ; bit 15 to 8 -&gt; veto pulse width</t>
+  </si>
+  <si>
+    <t>x0F327C</t>
+  </si>
+  <si>
+    <t>x000032</t>
   </si>
 </sst>
 </file>
@@ -1241,8 +1250,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B84" workbookViewId="0">
-      <selection activeCell="E103" sqref="E103"/>
+    <sheetView tabSelected="1" topLeftCell="B88" workbookViewId="0">
+      <selection activeCell="E106" sqref="E106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1961,10 +1970,10 @@
         <v>x21</v>
       </c>
       <c r="C40" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="D40" s="18" t="s">
         <v>230</v>
-      </c>
-      <c r="D40" s="18" t="s">
-        <v>231</v>
       </c>
       <c r="E40" s="18" t="s">
         <v>6</v>
@@ -3073,13 +3082,13 @@
         <v>224</v>
       </c>
       <c r="D102" s="5" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="E102" s="11" t="s">
         <v>235</v>
       </c>
       <c r="F102" s="5" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
@@ -3092,16 +3101,16 @@
         <v>x60</v>
       </c>
       <c r="C103" s="42" t="s">
+        <v>227</v>
+      </c>
+      <c r="D103" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="E103" s="42" t="s">
+        <v>237</v>
+      </c>
+      <c r="F103" s="5" t="s">
         <v>228</v>
-      </c>
-      <c r="D103" s="5" t="s">
-        <v>233</v>
-      </c>
-      <c r="E103" s="42" t="s">
-        <v>234</v>
-      </c>
-      <c r="F103" s="5" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
@@ -3113,9 +3122,15 @@
         <f t="shared" si="2"/>
         <v>x61</v>
       </c>
-      <c r="C104" s="11"/>
-      <c r="D104" s="5"/>
-      <c r="E104" s="11"/>
+      <c r="C104" s="11" t="s">
+        <v>233</v>
+      </c>
+      <c r="D104" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="E104" s="11" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105">

</xml_diff>

<commit_message>
fix ext. trig input / add trig delay function
</commit_message>
<xml_diff>
--- a/doc/firmware-register-map.xlsx
+++ b/doc/firmware-register-map.xlsx
@@ -1,30 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eric\Desktop\firmware-proto-beacon\firmware-proto-beacon\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eric\Desktop\projects\beacon\firmware_phased_protoBEACON\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{562CDECB-9F0B-4096-A819-6B4CD2A65585}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21390" windowHeight="7140"/>
+    <workbookView xWindow="-26190" yWindow="855" windowWidth="26970" windowHeight="14280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="241">
   <si>
     <t>Register Map</t>
   </si>
@@ -476,12 +483,6 @@
     <t>external trigger input config</t>
   </si>
   <si>
-    <t>if LSB=0, ext trig input acts as 'gate only' for scalers</t>
-  </si>
-  <si>
-    <t>(0) : accept external trig input to data manager; (1) : use gate generator; (8-23) : gate generator width</t>
-  </si>
-  <si>
     <t>x00FF00</t>
   </si>
   <si>
@@ -536,12 +537,6 @@
     <t>lower 16 bits -&gt; max trig hold off is 2^16 * 1/(31.25 MHz) = 2 millisecs</t>
   </si>
   <si>
-    <t>bit 0-&gt;enable; bit1-&gt;polarity; bit2-&gt; replace trigger output with 1Hz heartbeat pulse (debug use only) ; bits 8 to 15-&gt;width as specified by 31.25 MHz clock cycles</t>
-  </si>
-  <si>
-    <t>don't really care about this for protoBEACON</t>
-  </si>
-  <si>
     <t>current 32 bit register space: 8 bit address + 24 bit data (i.e. up to 256 24-bit registers)</t>
   </si>
   <si>
@@ -741,13 +736,87 @@
   </si>
   <si>
     <t>x000032</t>
+  </si>
+  <si>
+    <t>8/29/2019</t>
+  </si>
+  <si>
+    <t>&lt;&lt;----beacon proto round 2, edits shown in this color</t>
+  </si>
+  <si>
+    <t>bit 0-&gt;enable; bit1-&gt;polarity; bit2-&gt; replace trigger output with 1Hz heartbeat pulse (debug use only) ; bits 8 to 15-&gt;width as specified by 31.25 MHz clock cycles;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">don't really care about this for protoBEACON </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(0) : accept external trig input to data manager; </t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="5" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1) : use gate generator; (8-23) : gate generator width</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>bits 8-23: trig delay</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">if LSB=0, ext trig input acts as 'gate only' for scalers, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>trig_delay defines the delay between rising edge of ext. trig and sending trig to waveform capture. The total delay is given by trig_delay * 128 ns</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -795,6 +864,22 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="5" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -889,7 +974,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -966,8 +1051,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1247,11 +1337,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G175"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B88" workbookViewId="0">
-      <selection activeCell="E106" sqref="E106"/>
+    <sheetView tabSelected="1" topLeftCell="D82" workbookViewId="0">
+      <selection activeCell="F96" sqref="F96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1266,113 +1356,107 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="43" t="s">
-        <v>168</v>
-      </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
+      <c r="A1" s="44" t="s">
+        <v>166</v>
+      </c>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
       <c r="F3" s="6"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="44">
+      <c r="A4" s="45">
         <v>43305</v>
       </c>
-      <c r="B4" s="45"/>
+      <c r="B4" s="46"/>
       <c r="C4" s="1"/>
       <c r="D4" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
+    <row r="5" spans="1:7" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="47" t="s">
+        <v>235</v>
+      </c>
+      <c r="B5" s="47"/>
+      <c r="C5" s="48" t="s">
+        <v>236</v>
+      </c>
+      <c r="F5" s="5"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F6" s="7"/>
-      <c r="G6" s="2"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>0</v>
-      </c>
-      <c r="B7" s="26" t="str">
-        <f>"x" &amp; DEC2HEX(A7,2)</f>
-        <v>x00</v>
-      </c>
-      <c r="C7" t="s">
-        <v>93</v>
-      </c>
-      <c r="D7" s="25" t="s">
-        <v>95</v>
-      </c>
-      <c r="F7" s="13"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B8" s="26" t="str">
-        <f t="shared" ref="B8:B71" si="0">"x" &amp; DEC2HEX(A8,2)</f>
-        <v>x01</v>
+        <f>"x" &amp; DEC2HEX(A8,2)</f>
+        <v>x00</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" t="s">
-        <v>15</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="F8" s="13"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
-        <f>1+A8</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B9" s="26" t="str">
-        <f t="shared" si="0"/>
-        <v>x02</v>
+        <f t="shared" ref="B9:B72" si="0">"x" &amp; DEC2HEX(A9,2)</f>
+        <v>x01</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D9" t="s">
         <v>15</v>
@@ -1380,187 +1464,183 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
-        <f t="shared" ref="A10:A73" si="1">1+A9</f>
-        <v>3</v>
+        <f>1+A9</f>
+        <v>2</v>
       </c>
       <c r="B10" s="26" t="str">
         <f t="shared" si="0"/>
-        <v>x03</v>
+        <v>x02</v>
       </c>
       <c r="C10" t="s">
-        <v>59</v>
+        <v>16</v>
       </c>
       <c r="D10" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="5" t="s">
-        <v>110</v>
-      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
-        <f t="shared" si="1"/>
-        <v>4</v>
+        <f t="shared" ref="A11:A74" si="1">1+A10</f>
+        <v>3</v>
       </c>
       <c r="B11" s="26" t="str">
         <f t="shared" si="0"/>
-        <v>x04</v>
+        <v>x03</v>
       </c>
       <c r="C11" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
       <c r="D11" t="s">
-        <v>51</v>
+        <v>15</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>76</v>
+        <v>110</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B12" s="26" t="str">
         <f t="shared" si="0"/>
-        <v>x05</v>
+        <v>x04</v>
       </c>
       <c r="C12" t="s">
-        <v>36</v>
-      </c>
-      <c r="D12" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" t="s">
         <v>51</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>37</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="B13" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v>x05</v>
+      </c>
+      <c r="C13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="B13" s="26" t="str">
+      <c r="B14" s="26" t="str">
         <f t="shared" si="0"/>
         <v>x06</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>115</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="D14" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F14" s="5" t="s">
         <v>117</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="B14" s="26" t="str">
-        <f t="shared" si="0"/>
-        <v>x07</v>
-      </c>
-      <c r="C14" t="s">
-        <v>55</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B15" s="26" t="str">
         <f t="shared" si="0"/>
-        <v>x08</v>
+        <v>x07</v>
       </c>
       <c r="C15" t="s">
-        <v>79</v>
+        <v>55</v>
       </c>
       <c r="D15" s="11" t="s">
         <v>15</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B16" s="26" t="str">
         <f t="shared" si="0"/>
-        <v>x09</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>97</v>
+        <v>x08</v>
+      </c>
+      <c r="C16" t="s">
+        <v>79</v>
       </c>
       <c r="D16" s="11" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="14">
+      <c r="F16" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="B17" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v>x09</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="14">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="B17" s="27" t="str">
+      <c r="B18" s="27" t="str">
         <f t="shared" si="0"/>
         <v>x0A</v>
       </c>
-      <c r="C17" s="15" t="s">
+      <c r="C18" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="D17" s="15" t="s">
+      <c r="D18" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="E17" s="15" t="s">
+      <c r="E18" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="F17" s="16" t="s">
+      <c r="F18" s="16" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="17">
-        <f t="shared" si="1"/>
-        <v>11</v>
-      </c>
-      <c r="B18" s="28" t="str">
-        <f t="shared" si="0"/>
-        <v>x0B</v>
-      </c>
-      <c r="C18" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="D18" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="E18" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="F18" s="19"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="17">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B19" s="28" t="str">
         <f t="shared" si="0"/>
-        <v>x0C</v>
+        <v>x0B</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D19" s="18" t="s">
         <v>61</v>
@@ -1573,14 +1653,14 @@
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="17">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B20" s="28" t="str">
         <f t="shared" si="0"/>
-        <v>x0D</v>
+        <v>x0C</v>
       </c>
       <c r="C20" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D20" s="18" t="s">
         <v>61</v>
@@ -1593,14 +1673,14 @@
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="17">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B21" s="28" t="str">
         <f t="shared" si="0"/>
-        <v>x0E</v>
+        <v>x0D</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D21" s="18" t="s">
         <v>61</v>
@@ -1613,14 +1693,14 @@
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="17">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B22" s="28" t="str">
         <f t="shared" si="0"/>
-        <v>x0F</v>
+        <v>x0E</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D22" s="18" t="s">
         <v>61</v>
@@ -1633,14 +1713,14 @@
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="17">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B23" s="28" t="str">
         <f t="shared" si="0"/>
-        <v>x10</v>
+        <v>x0F</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D23" s="18" t="s">
         <v>61</v>
@@ -1648,21 +1728,19 @@
       <c r="E23" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="F23" s="19" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="F23" s="19"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="17">
         <f t="shared" si="1"/>
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B24" s="28" t="str">
         <f t="shared" si="0"/>
-        <v>x11</v>
+        <v>x10</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>200</v>
+        <v>69</v>
       </c>
       <c r="D24" s="18" t="s">
         <v>61</v>
@@ -1671,20 +1749,20 @@
         <v>6</v>
       </c>
       <c r="F24" s="19" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="17">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B25" s="28" t="str">
         <f t="shared" si="0"/>
-        <v>x12</v>
+        <v>x11</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>71</v>
+        <v>196</v>
       </c>
       <c r="D25" s="18" t="s">
         <v>61</v>
@@ -1693,20 +1771,20 @@
         <v>6</v>
       </c>
       <c r="F25" s="19" t="s">
-        <v>221</v>
+        <v>197</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="17">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B26" s="28" t="str">
         <f t="shared" si="0"/>
-        <v>x13</v>
+        <v>x12</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D26" s="18" t="s">
         <v>61</v>
@@ -1714,19 +1792,21 @@
       <c r="E26" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="F26" s="19"/>
+      <c r="F26" s="19" t="s">
+        <v>217</v>
+      </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="17">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B27" s="28" t="str">
         <f t="shared" si="0"/>
-        <v>x14</v>
-      </c>
-      <c r="C27" s="22" t="s">
-        <v>162</v>
+        <v>x13</v>
+      </c>
+      <c r="C27" s="18" t="s">
+        <v>72</v>
       </c>
       <c r="D27" s="18" t="s">
         <v>61</v>
@@ -1734,21 +1814,19 @@
       <c r="E27" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="F27" s="19" t="s">
-        <v>163</v>
-      </c>
+      <c r="F27" s="19"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="17">
         <f t="shared" si="1"/>
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B28" s="28" t="str">
         <f t="shared" si="0"/>
-        <v>x15</v>
+        <v>x14</v>
       </c>
       <c r="C28" s="22" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="D28" s="18" t="s">
         <v>61</v>
@@ -1757,42 +1835,42 @@
         <v>6</v>
       </c>
       <c r="F28" s="19" t="s">
-        <v>202</v>
+        <v>161</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="17">
         <f t="shared" si="1"/>
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B29" s="28" t="str">
         <f t="shared" si="0"/>
-        <v>x16</v>
+        <v>x15</v>
       </c>
       <c r="C29" s="22" t="s">
-        <v>205</v>
-      </c>
-      <c r="D29" s="22" t="s">
+        <v>162</v>
+      </c>
+      <c r="D29" s="18" t="s">
         <v>61</v>
       </c>
       <c r="E29" s="18" t="s">
         <v>6</v>
       </c>
       <c r="F29" s="19" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="17">
         <f t="shared" si="1"/>
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B30" s="28" t="str">
         <f t="shared" si="0"/>
-        <v>x17</v>
+        <v>x16</v>
       </c>
       <c r="C30" s="22" t="s">
-        <v>217</v>
+        <v>201</v>
       </c>
       <c r="D30" s="22" t="s">
         <v>61</v>
@@ -1801,20 +1879,20 @@
         <v>6</v>
       </c>
       <c r="F30" s="19" t="s">
-        <v>218</v>
+        <v>202</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="17">
         <f t="shared" si="1"/>
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B31" s="28" t="str">
         <f t="shared" si="0"/>
-        <v>x18</v>
+        <v>x17</v>
       </c>
       <c r="C31" s="22" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="D31" s="22" t="s">
         <v>61</v>
@@ -1823,20 +1901,20 @@
         <v>6</v>
       </c>
       <c r="F31" s="19" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="17">
         <f t="shared" si="1"/>
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B32" s="28" t="str">
         <f t="shared" si="0"/>
-        <v>x19</v>
+        <v>x18</v>
       </c>
       <c r="C32" s="22" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="D32" s="22" t="s">
         <v>61</v>
@@ -1845,33 +1923,39 @@
         <v>6</v>
       </c>
       <c r="F32" s="19" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="17">
         <f t="shared" si="1"/>
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B33" s="28" t="str">
         <f t="shared" si="0"/>
-        <v>x1A</v>
-      </c>
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
+        <v>x19</v>
+      </c>
+      <c r="C33" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="D33" s="22" t="s">
+        <v>61</v>
+      </c>
       <c r="E33" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="F33" s="19"/>
+      <c r="F33" s="19" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="17">
         <f t="shared" si="1"/>
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B34" s="28" t="str">
         <f t="shared" si="0"/>
-        <v>x1B</v>
+        <v>x1A</v>
       </c>
       <c r="C34" s="18"/>
       <c r="D34" s="18"/>
@@ -1883,11 +1967,11 @@
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="17">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B35" s="28" t="str">
         <f t="shared" si="0"/>
-        <v>x1C</v>
+        <v>x1B</v>
       </c>
       <c r="C35" s="18"/>
       <c r="D35" s="18"/>
@@ -1899,11 +1983,11 @@
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="17">
         <f t="shared" si="1"/>
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B36" s="28" t="str">
         <f t="shared" si="0"/>
-        <v>x1D</v>
+        <v>x1C</v>
       </c>
       <c r="C36" s="18"/>
       <c r="D36" s="18"/>
@@ -1915,11 +1999,11 @@
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="17">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B37" s="28" t="str">
         <f t="shared" si="0"/>
-        <v>x1E</v>
+        <v>x1D</v>
       </c>
       <c r="C37" s="18"/>
       <c r="D37" s="18"/>
@@ -1931,11 +2015,11 @@
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="17">
         <f t="shared" si="1"/>
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B38" s="28" t="str">
         <f t="shared" si="0"/>
-        <v>x1F</v>
+        <v>x1E</v>
       </c>
       <c r="C38" s="18"/>
       <c r="D38" s="18"/>
@@ -1947,11 +2031,11 @@
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="17">
         <f t="shared" si="1"/>
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B39" s="28" t="str">
         <f t="shared" si="0"/>
-        <v>x20</v>
+        <v>x1F</v>
       </c>
       <c r="C39" s="18"/>
       <c r="D39" s="18"/>
@@ -1963,75 +2047,72 @@
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="17">
         <f t="shared" si="1"/>
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B40" s="28" t="str">
         <f t="shared" si="0"/>
-        <v>x21</v>
-      </c>
-      <c r="C40" s="18" t="s">
-        <v>229</v>
-      </c>
-      <c r="D40" s="18" t="s">
-        <v>230</v>
-      </c>
+        <v>x20</v>
+      </c>
+      <c r="C40" s="18"/>
+      <c r="D40" s="18"/>
       <c r="E40" s="18" t="s">
         <v>6</v>
       </c>
       <c r="F40" s="19"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="20">
+      <c r="A41" s="17">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="B41" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v>x21</v>
+      </c>
+      <c r="C41" s="18" t="s">
+        <v>225</v>
+      </c>
+      <c r="D41" s="18" t="s">
+        <v>226</v>
+      </c>
+      <c r="E41" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="F41" s="19"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="20">
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
-      <c r="B41" s="29" t="str">
+      <c r="B42" s="29" t="str">
         <f t="shared" si="0"/>
         <v>x22</v>
       </c>
-      <c r="C41" s="21" t="s">
-        <v>219</v>
-      </c>
-      <c r="D41" s="21" t="s">
+      <c r="C42" s="21" t="s">
+        <v>215</v>
+      </c>
+      <c r="D42" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="E41" s="21" t="s">
+      <c r="E42" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="F41" s="41" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <f t="shared" si="1"/>
-        <v>35</v>
-      </c>
-      <c r="B42" s="26" t="str">
-        <f t="shared" si="0"/>
-        <v>x23</v>
-      </c>
-      <c r="C42" s="22" t="s">
-        <v>81</v>
-      </c>
-      <c r="D42" s="22" t="s">
-        <v>87</v>
-      </c>
-      <c r="F42" s="23" t="s">
-        <v>85</v>
+      <c r="F42" s="41" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
         <f t="shared" si="1"/>
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B43" s="26" t="str">
         <f t="shared" si="0"/>
-        <v>x24</v>
+        <v>x23</v>
       </c>
       <c r="C43" s="22" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D43" s="22" t="s">
         <v>87</v>
@@ -2043,14 +2124,14 @@
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44">
         <f t="shared" si="1"/>
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B44" s="26" t="str">
         <f t="shared" si="0"/>
-        <v>x25</v>
+        <v>x24</v>
       </c>
       <c r="C44" s="22" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D44" s="22" t="s">
         <v>87</v>
@@ -2062,14 +2143,14 @@
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
         <f t="shared" si="1"/>
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B45" s="26" t="str">
         <f t="shared" si="0"/>
-        <v>x26</v>
+        <v>x25</v>
       </c>
       <c r="C45" s="22" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D45" s="22" t="s">
         <v>87</v>
@@ -2081,224 +2162,221 @@
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
         <f t="shared" si="1"/>
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B46" s="26" t="str">
         <f t="shared" si="0"/>
-        <v>x27</v>
+        <v>x26</v>
       </c>
       <c r="C46" s="22" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="D46" s="22" t="s">
-        <v>101</v>
-      </c>
-      <c r="E46" t="s">
-        <v>6</v>
-      </c>
-      <c r="F46" s="5" t="s">
-        <v>100</v>
+        <v>87</v>
+      </c>
+      <c r="F46" s="23" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47">
         <f t="shared" si="1"/>
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B47" s="26" t="str">
         <f t="shared" si="0"/>
-        <v>x28</v>
-      </c>
-      <c r="C47" t="s">
-        <v>153</v>
-      </c>
-      <c r="D47" t="s">
-        <v>154</v>
+        <v>x27</v>
+      </c>
+      <c r="C47" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="D47" s="22" t="s">
+        <v>101</v>
       </c>
       <c r="E47" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="F47" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48">
         <f t="shared" si="1"/>
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B48" s="26" t="str">
         <f t="shared" si="0"/>
-        <v>x29</v>
+        <v>x28</v>
       </c>
       <c r="C48" t="s">
-        <v>58</v>
+        <v>151</v>
       </c>
       <c r="D48" t="s">
-        <v>198</v>
+        <v>152</v>
       </c>
       <c r="E48" t="s">
         <v>6</v>
       </c>
-      <c r="F48" s="5" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A49">
         <f t="shared" si="1"/>
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B49" s="26" t="str">
         <f t="shared" si="0"/>
-        <v>x2A</v>
+        <v>x29</v>
       </c>
       <c r="C49" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="D49" t="s">
-        <v>39</v>
+        <v>194</v>
       </c>
       <c r="E49" t="s">
         <v>6</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>40</v>
+        <v>195</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50">
         <f t="shared" si="1"/>
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B50" s="26" t="str">
         <f t="shared" si="0"/>
-        <v>x2B</v>
+        <v>x2A</v>
+      </c>
+      <c r="C50" t="s">
+        <v>38</v>
+      </c>
+      <c r="D50" t="s">
+        <v>39</v>
+      </c>
+      <c r="E50" t="s">
+        <v>6</v>
+      </c>
+      <c r="F50" s="5" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51">
         <f t="shared" si="1"/>
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B51" s="26" t="str">
         <f t="shared" si="0"/>
-        <v>x2C</v>
-      </c>
-      <c r="C51" t="s">
-        <v>155</v>
-      </c>
-      <c r="D51" t="s">
-        <v>158</v>
-      </c>
-      <c r="F51" s="5" t="s">
-        <v>157</v>
+        <v>x2B</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52">
         <f t="shared" si="1"/>
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B52" s="26" t="str">
         <f t="shared" si="0"/>
-        <v>x2D</v>
-      </c>
-      <c r="C52" s="32" t="s">
+        <v>x2C</v>
+      </c>
+      <c r="C52" t="s">
+        <v>153</v>
+      </c>
+      <c r="D52" t="s">
         <v>156</v>
       </c>
-      <c r="D52" s="32" t="s">
-        <v>158</v>
-      </c>
       <c r="F52" s="5" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53">
         <f t="shared" si="1"/>
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B53" s="26" t="str">
         <f t="shared" si="0"/>
-        <v>x2E</v>
+        <v>x2D</v>
+      </c>
+      <c r="C53" s="32" t="s">
+        <v>154</v>
+      </c>
+      <c r="D53" s="32" t="s">
+        <v>156</v>
+      </c>
+      <c r="F53" s="5" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54">
         <f t="shared" si="1"/>
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B54" s="26" t="str">
         <f t="shared" si="0"/>
-        <v>x2F</v>
+        <v>x2E</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55">
         <f t="shared" si="1"/>
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B55" s="26" t="str">
         <f t="shared" si="0"/>
-        <v>x30</v>
-      </c>
-      <c r="C55" t="s">
-        <v>43</v>
-      </c>
-      <c r="D55" t="s">
-        <v>56</v>
-      </c>
-      <c r="E55" t="s">
-        <v>57</v>
-      </c>
-      <c r="F55" s="5" t="s">
-        <v>112</v>
+        <v>x2F</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56">
         <f t="shared" si="1"/>
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B56" s="26" t="str">
         <f t="shared" si="0"/>
-        <v>x31</v>
+        <v>x30</v>
+      </c>
+      <c r="C56" t="s">
+        <v>43</v>
+      </c>
+      <c r="D56" t="s">
+        <v>56</v>
+      </c>
+      <c r="E56" t="s">
+        <v>57</v>
+      </c>
+      <c r="F56" s="5" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57">
         <f t="shared" si="1"/>
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B57" s="26" t="str">
         <f t="shared" si="0"/>
-        <v>x32</v>
-      </c>
-      <c r="C57" t="s">
-        <v>19</v>
-      </c>
-      <c r="D57" t="s">
-        <v>21</v>
-      </c>
-      <c r="E57" t="s">
-        <v>6</v>
-      </c>
-      <c r="F57" s="5" t="s">
-        <v>111</v>
+        <v>x31</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58">
         <f t="shared" si="1"/>
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B58" s="26" t="str">
         <f t="shared" si="0"/>
-        <v>x33</v>
+        <v>x32</v>
       </c>
       <c r="C58" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D58" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E58" t="s">
         <v>6</v>
@@ -2310,17 +2388,17 @@
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59">
         <f t="shared" si="1"/>
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B59" s="26" t="str">
         <f t="shared" si="0"/>
-        <v>x34</v>
+        <v>x33</v>
       </c>
       <c r="C59" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D59" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E59" t="s">
         <v>6</v>
@@ -2332,81 +2410,84 @@
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60">
         <f t="shared" si="1"/>
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B60" s="26" t="str">
         <f t="shared" si="0"/>
-        <v>x35</v>
+        <v>x34</v>
       </c>
       <c r="C60" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D60" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="E60" t="s">
         <v>6</v>
       </c>
+      <c r="F60" s="5" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61">
         <f t="shared" si="1"/>
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B61" s="26" t="str">
         <f t="shared" si="0"/>
-        <v>x36</v>
+        <v>x35</v>
+      </c>
+      <c r="C61" t="s">
+        <v>20</v>
+      </c>
+      <c r="D61" t="s">
+        <v>11</v>
+      </c>
+      <c r="E61" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62">
         <f t="shared" si="1"/>
+        <v>54</v>
+      </c>
+      <c r="B62" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v>x36</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <f t="shared" si="1"/>
         <v>55</v>
       </c>
-      <c r="B62" s="26" t="str">
+      <c r="B63" s="26" t="str">
         <f t="shared" si="0"/>
         <v>x37</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C63" t="s">
         <v>26</v>
       </c>
-      <c r="D62" t="s">
+      <c r="D63" t="s">
         <v>52</v>
       </c>
-      <c r="E62" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A63">
-        <f t="shared" si="1"/>
-        <v>56</v>
-      </c>
-      <c r="B63" s="26" t="str">
-        <f t="shared" si="0"/>
-        <v>x38</v>
-      </c>
-      <c r="C63" t="s">
-        <v>28</v>
-      </c>
-      <c r="D63" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="E63" s="3" t="s">
+      <c r="E63" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A64">
         <f t="shared" si="1"/>
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B64" s="26" t="str">
         <f t="shared" si="0"/>
-        <v>x39</v>
-      </c>
-      <c r="C64" s="3" t="s">
-        <v>29</v>
+        <v>x38</v>
+      </c>
+      <c r="C64" t="s">
+        <v>28</v>
       </c>
       <c r="D64" s="5" t="s">
         <v>106</v>
@@ -2418,14 +2499,14 @@
     <row r="65" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A65">
         <f t="shared" si="1"/>
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B65" s="26" t="str">
         <f t="shared" si="0"/>
-        <v>x3A</v>
+        <v>x39</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D65" s="5" t="s">
         <v>106</v>
@@ -2437,14 +2518,14 @@
     <row r="66" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A66">
         <f t="shared" si="1"/>
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B66" s="26" t="str">
         <f t="shared" si="0"/>
-        <v>x3B</v>
+        <v>x3A</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D66" s="5" t="s">
         <v>106</v>
@@ -2453,56 +2534,63 @@
         <v>6</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A67">
         <f t="shared" si="1"/>
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B67" s="26" t="str">
         <f t="shared" si="0"/>
-        <v>x3C</v>
-      </c>
-      <c r="C67" t="s">
-        <v>41</v>
-      </c>
-      <c r="D67" t="s">
-        <v>42</v>
-      </c>
-      <c r="E67" t="s">
+        <v>x3B</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D67" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="E67" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68">
         <f t="shared" si="1"/>
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B68" s="26" t="str">
         <f t="shared" si="0"/>
-        <v>x3D</v>
-      </c>
-      <c r="D68" s="5"/>
+        <v>x3C</v>
+      </c>
+      <c r="C68" t="s">
+        <v>41</v>
+      </c>
+      <c r="D68" t="s">
+        <v>42</v>
+      </c>
+      <c r="E68" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69">
         <f t="shared" si="1"/>
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B69" s="26" t="str">
         <f t="shared" si="0"/>
-        <v>x3E</v>
-      </c>
-      <c r="C69" s="34"/>
+        <v>x3D</v>
+      </c>
       <c r="D69" s="5"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70">
         <f t="shared" si="1"/>
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B70" s="26" t="str">
         <f t="shared" si="0"/>
-        <v>x3F</v>
+        <v>x3E</v>
       </c>
       <c r="C70" s="34"/>
       <c r="D70" s="5"/>
@@ -2510,36 +2598,29 @@
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71">
         <f t="shared" si="1"/>
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B71" s="26" t="str">
         <f t="shared" si="0"/>
-        <v>x40</v>
-      </c>
-      <c r="C71" t="s">
-        <v>9</v>
-      </c>
-      <c r="D71" t="s">
-        <v>8</v>
-      </c>
-      <c r="E71" t="s">
-        <v>7</v>
-      </c>
+        <v>x3F</v>
+      </c>
+      <c r="C71" s="34"/>
+      <c r="D71" s="5"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72">
         <f t="shared" si="1"/>
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B72" s="26" t="str">
-        <f t="shared" ref="B72:B135" si="2">"x" &amp; DEC2HEX(A72,2)</f>
-        <v>x41</v>
+        <f t="shared" si="0"/>
+        <v>x40</v>
       </c>
       <c r="C72" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D72" t="s">
-        <v>78</v>
+        <v>8</v>
       </c>
       <c r="E72" t="s">
         <v>7</v>
@@ -2548,484 +2629,490 @@
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73">
         <f t="shared" si="1"/>
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B73" s="26" t="str">
-        <f t="shared" si="2"/>
-        <v>x42</v>
+        <f t="shared" ref="B73:B136" si="2">"x" &amp; DEC2HEX(A73,2)</f>
+        <v>x41</v>
       </c>
       <c r="C73" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="D73" t="s">
-        <v>45</v>
+        <v>78</v>
       </c>
       <c r="E73" t="s">
         <v>7</v>
       </c>
-      <c r="F73" s="5" t="s">
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <f t="shared" si="1"/>
+        <v>66</v>
+      </c>
+      <c r="B74" s="26" t="str">
+        <f t="shared" si="2"/>
+        <v>x42</v>
+      </c>
+      <c r="C74" t="s">
+        <v>34</v>
+      </c>
+      <c r="D74" t="s">
+        <v>45</v>
+      </c>
+      <c r="E74" t="s">
+        <v>7</v>
+      </c>
+      <c r="F74" s="5" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="74" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="8">
-        <f t="shared" ref="A74:A134" si="3">1+A73</f>
-        <v>67</v>
-      </c>
-      <c r="B74" s="26" t="str">
-        <f t="shared" si="2"/>
-        <v>x43</v>
-      </c>
-      <c r="F74" s="10"/>
     </row>
     <row r="75" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="8">
+        <f t="shared" ref="A75:A135" si="3">1+A74</f>
+        <v>67</v>
+      </c>
+      <c r="B75" s="26" t="str">
+        <f t="shared" si="2"/>
+        <v>x43</v>
+      </c>
+      <c r="F75" s="10"/>
+    </row>
+    <row r="76" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="8">
         <f t="shared" si="3"/>
         <v>68</v>
       </c>
-      <c r="B75" s="26" t="str">
+      <c r="B76" s="26" t="str">
         <f t="shared" si="2"/>
         <v>x44</v>
       </c>
-      <c r="F75" s="10"/>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" s="8">
+      <c r="F76" s="10"/>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" s="8">
         <f t="shared" si="3"/>
         <v>69</v>
       </c>
-      <c r="B76" s="26" t="str">
+      <c r="B77" s="26" t="str">
         <f t="shared" si="2"/>
         <v>x45</v>
       </c>
-      <c r="C76" s="8" t="s">
+      <c r="C77" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="D76" s="8" t="s">
+      <c r="D77" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="E76" t="s">
+      <c r="E77" t="s">
         <v>7</v>
       </c>
-      <c r="F76" s="5" t="s">
+      <c r="F77" s="5" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="77" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="8">
+    <row r="78" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="8">
         <f t="shared" si="3"/>
         <v>70</v>
       </c>
-      <c r="B77" s="26" t="str">
+      <c r="B78" s="26" t="str">
         <f t="shared" si="2"/>
         <v>x46</v>
       </c>
-      <c r="F77" s="10"/>
-    </row>
-    <row r="78" spans="1:6" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A78" s="8">
+      <c r="F78" s="10"/>
+    </row>
+    <row r="79" spans="1:6" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A79" s="8">
         <f t="shared" si="3"/>
         <v>71</v>
       </c>
-      <c r="B78" s="26" t="str">
+      <c r="B79" s="26" t="str">
         <f t="shared" si="2"/>
         <v>x47</v>
       </c>
-      <c r="C78" s="12" t="s">
+      <c r="C79" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D78" s="12" t="s">
+      <c r="D79" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E78" s="12" t="s">
+      <c r="E79" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="F78" s="5" t="s">
+      <c r="F79" s="5" t="s">
         <v>96</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" s="8">
-        <f t="shared" si="3"/>
-        <v>72</v>
-      </c>
-      <c r="B79" s="26" t="str">
-        <f t="shared" si="2"/>
-        <v>x48</v>
-      </c>
-      <c r="C79" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D79" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E79" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F79" s="24" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="8">
         <f t="shared" si="3"/>
+        <v>72</v>
+      </c>
+      <c r="B80" s="26" t="str">
+        <f t="shared" si="2"/>
+        <v>x48</v>
+      </c>
+      <c r="C80" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D80" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E80" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F80" s="24" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" s="8">
+        <f t="shared" si="3"/>
         <v>73</v>
       </c>
-      <c r="B80" s="26" t="str">
+      <c r="B81" s="26" t="str">
         <f t="shared" si="2"/>
         <v>x49</v>
       </c>
-      <c r="E80" s="4"/>
-    </row>
-    <row r="81" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="8">
+      <c r="E81" s="4"/>
+    </row>
+    <row r="82" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="8">
         <f t="shared" si="3"/>
         <v>74</v>
       </c>
-      <c r="B81" s="26" t="str">
+      <c r="B82" s="26" t="str">
         <f t="shared" si="2"/>
         <v>x4A</v>
       </c>
-      <c r="C81" s="8"/>
-      <c r="D81" s="12"/>
-      <c r="F81" s="10"/>
-    </row>
-    <row r="82" spans="1:6" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A82" s="8">
+      <c r="C82" s="8"/>
+      <c r="D82" s="12"/>
+      <c r="F82" s="10"/>
+    </row>
+    <row r="83" spans="1:6" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A83" s="8">
         <f t="shared" si="3"/>
         <v>75</v>
       </c>
-      <c r="B82" s="26" t="str">
+      <c r="B83" s="26" t="str">
         <f t="shared" si="2"/>
         <v>x4B</v>
       </c>
-      <c r="C82" s="8" t="s">
+      <c r="C83" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="D82" s="24" t="s">
-        <v>151</v>
-      </c>
-      <c r="E82" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="F82" s="33" t="s">
+      <c r="D83" s="24" t="s">
+        <v>239</v>
+      </c>
+      <c r="E83" s="8" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="83" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A83">
+      <c r="F83" s="33" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A84">
         <f t="shared" si="3"/>
         <v>76</v>
       </c>
-      <c r="B83" s="26" t="str">
+      <c r="B84" s="26" t="str">
         <f t="shared" si="2"/>
         <v>x4C</v>
       </c>
-      <c r="C83" t="s">
+      <c r="C84" t="s">
         <v>50</v>
       </c>
-      <c r="D83" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="E83" t="s">
+      <c r="D84" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="E84" t="s">
         <v>113</v>
       </c>
-      <c r="F83" s="5" t="s">
+      <c r="F84" s="5" t="s">
         <v>114</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84">
-        <f t="shared" si="3"/>
-        <v>77</v>
-      </c>
-      <c r="B84" s="26" t="str">
-        <f t="shared" si="2"/>
-        <v>x4D</v>
-      </c>
-      <c r="C84" t="s">
-        <v>103</v>
-      </c>
-      <c r="D84" t="s">
-        <v>104</v>
-      </c>
-      <c r="E84" t="s">
-        <v>7</v>
-      </c>
-      <c r="F84" s="5" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85">
         <f t="shared" si="3"/>
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B85" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>x4E</v>
+        <v>x4D</v>
       </c>
       <c r="C85" t="s">
-        <v>53</v>
+        <v>103</v>
       </c>
       <c r="D85" t="s">
-        <v>54</v>
+        <v>104</v>
       </c>
       <c r="E85" t="s">
         <v>7</v>
       </c>
       <c r="F85" s="5" t="s">
-        <v>77</v>
+        <v>105</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86">
         <f t="shared" si="3"/>
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B86" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>x4F</v>
+        <v>x4E</v>
       </c>
       <c r="C86" t="s">
-        <v>166</v>
+        <v>53</v>
       </c>
       <c r="D86" t="s">
-        <v>160</v>
+        <v>54</v>
       </c>
       <c r="E86" t="s">
         <v>7</v>
       </c>
+      <c r="F86" s="5" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87">
         <f t="shared" si="3"/>
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B87" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>x50</v>
+        <v>x4F</v>
       </c>
       <c r="C87" t="s">
-        <v>47</v>
+        <v>164</v>
       </c>
       <c r="D87" t="s">
-        <v>49</v>
+        <v>158</v>
       </c>
       <c r="E87" t="s">
-        <v>75</v>
-      </c>
-      <c r="F87" s="5" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88">
         <f t="shared" si="3"/>
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B88" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>x51</v>
+        <v>x50</v>
       </c>
       <c r="C88" t="s">
-        <v>74</v>
-      </c>
-      <c r="D88" s="5" t="s">
-        <v>121</v>
+        <v>47</v>
+      </c>
+      <c r="D88" t="s">
+        <v>49</v>
       </c>
       <c r="E88" t="s">
-        <v>210</v>
+        <v>75</v>
       </c>
       <c r="F88" s="5" t="s">
-        <v>169</v>
+        <v>48</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89">
         <f t="shared" si="3"/>
+        <v>81</v>
+      </c>
+      <c r="B89" s="26" t="str">
+        <f t="shared" si="2"/>
+        <v>x51</v>
+      </c>
+      <c r="C89" t="s">
+        <v>74</v>
+      </c>
+      <c r="D89" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="E89" t="s">
+        <v>206</v>
+      </c>
+      <c r="F89" s="5" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <f t="shared" si="3"/>
         <v>82</v>
       </c>
-      <c r="B89" s="26" t="str">
+      <c r="B90" s="26" t="str">
         <f t="shared" si="2"/>
         <v>x52</v>
       </c>
-      <c r="C89" t="s">
+      <c r="C90" t="s">
         <v>148</v>
       </c>
-      <c r="D89" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="E89" t="s">
-        <v>207</v>
-      </c>
-      <c r="F89" s="5" t="s">
+      <c r="D90" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="E90" t="s">
+        <v>203</v>
+      </c>
+      <c r="F90" s="5" t="s">
         <v>102</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A90">
-        <f t="shared" si="3"/>
-        <v>83</v>
-      </c>
-      <c r="B90" s="26" t="str">
-        <f t="shared" si="2"/>
-        <v>x53</v>
-      </c>
-      <c r="C90" t="s">
-        <v>98</v>
-      </c>
-      <c r="D90" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="E90" t="s">
-        <v>159</v>
-      </c>
-      <c r="F90" s="5" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="91" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A91">
         <f t="shared" si="3"/>
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B91" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>x54</v>
+        <v>x53</v>
       </c>
       <c r="C91" t="s">
-        <v>107</v>
-      </c>
-      <c r="D91" t="s">
-        <v>108</v>
+        <v>98</v>
+      </c>
+      <c r="D91" s="5" t="s">
+        <v>237</v>
       </c>
       <c r="E91" t="s">
-        <v>7</v>
-      </c>
-      <c r="F91" s="5" t="s">
-        <v>109</v>
+        <v>157</v>
+      </c>
+      <c r="F91" s="24" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="92" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A92">
         <f t="shared" si="3"/>
+        <v>84</v>
+      </c>
+      <c r="B92" s="26" t="str">
+        <f t="shared" si="2"/>
+        <v>x54</v>
+      </c>
+      <c r="C92" t="s">
+        <v>107</v>
+      </c>
+      <c r="D92" t="s">
+        <v>108</v>
+      </c>
+      <c r="E92" t="s">
+        <v>7</v>
+      </c>
+      <c r="F92" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <f t="shared" si="3"/>
         <v>85</v>
       </c>
-      <c r="B92" s="26" t="str">
+      <c r="B93" s="26" t="str">
         <f t="shared" si="2"/>
         <v>x55</v>
       </c>
-      <c r="C92" t="s">
+      <c r="C93" t="s">
         <v>122</v>
       </c>
-      <c r="D92" s="5" t="s">
+      <c r="D93" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="E92" s="11" t="s">
+      <c r="E93" s="11" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A93">
-        <f t="shared" si="3"/>
-        <v>86</v>
-      </c>
-      <c r="B93" s="26" t="str">
-        <f t="shared" si="2"/>
-        <v>x56</v>
-      </c>
-      <c r="C93" s="39"/>
-      <c r="D93" s="40"/>
-      <c r="E93" s="39"/>
-      <c r="F93" s="40"/>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94">
         <f t="shared" si="3"/>
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B94" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>x57</v>
-      </c>
-      <c r="C94" s="39"/>
-      <c r="D94" s="40"/>
+        <v>x56</v>
+      </c>
+      <c r="C94" s="35"/>
+      <c r="D94" s="24"/>
       <c r="E94" s="39"/>
       <c r="F94" s="40"/>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95">
         <f t="shared" si="3"/>
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B95" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>x58</v>
-      </c>
-      <c r="C95" s="11" t="s">
-        <v>203</v>
-      </c>
-      <c r="D95" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="E95" s="11" t="s">
-        <v>7</v>
-      </c>
+        <v>x57</v>
+      </c>
+      <c r="C95" s="39"/>
+      <c r="D95" s="40"/>
+      <c r="E95" s="39"/>
+      <c r="F95" s="40"/>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96">
         <f t="shared" si="3"/>
+        <v>88</v>
+      </c>
+      <c r="B96" s="26" t="str">
+        <f t="shared" si="2"/>
+        <v>x58</v>
+      </c>
+      <c r="C96" s="11" t="s">
+        <v>199</v>
+      </c>
+      <c r="D96" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="E96" s="11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <f t="shared" si="3"/>
         <v>89</v>
       </c>
-      <c r="B96" s="26" t="str">
+      <c r="B97" s="26" t="str">
         <f t="shared" si="2"/>
         <v>x59</v>
       </c>
-      <c r="C96" s="11"/>
-      <c r="D96" s="5"/>
-      <c r="E96" s="11"/>
-    </row>
-    <row r="97" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A97">
+      <c r="C97" s="11"/>
+      <c r="D97" s="5"/>
+      <c r="E97" s="11"/>
+    </row>
+    <row r="98" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A98">
         <f t="shared" si="3"/>
         <v>90</v>
       </c>
-      <c r="B97" s="26" t="str">
+      <c r="B98" s="26" t="str">
         <f t="shared" si="2"/>
         <v>x5A</v>
       </c>
-      <c r="C97" s="11" t="s">
-        <v>208</v>
-      </c>
-      <c r="D97" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="E97" s="11" t="s">
+      <c r="C98" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="D98" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="E98" s="11" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A98">
-        <f t="shared" si="3"/>
-        <v>91</v>
-      </c>
-      <c r="B98" s="26" t="str">
-        <f t="shared" si="2"/>
-        <v>x5B</v>
-      </c>
-      <c r="C98" s="11"/>
-      <c r="D98" s="5"/>
-      <c r="E98" s="11"/>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99">
         <f t="shared" si="3"/>
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B99" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>x5C</v>
+        <v>x5B</v>
       </c>
       <c r="C99" s="11"/>
       <c r="D99" s="5"/>
@@ -3034,80 +3121,71 @@
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100">
         <f t="shared" si="3"/>
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B100" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>x5D</v>
-      </c>
-      <c r="C100" s="11" t="s">
-        <v>211</v>
-      </c>
-      <c r="D100" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="E100" s="11" t="s">
-        <v>213</v>
-      </c>
+        <v>x5C</v>
+      </c>
+      <c r="C100" s="11"/>
+      <c r="D100" s="5"/>
+      <c r="E100" s="11"/>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101">
         <f t="shared" si="3"/>
+        <v>93</v>
+      </c>
+      <c r="B101" s="26" t="str">
+        <f t="shared" si="2"/>
+        <v>x5D</v>
+      </c>
+      <c r="C101" s="11" t="s">
+        <v>207</v>
+      </c>
+      <c r="D101" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="E101" s="11" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <f t="shared" si="3"/>
         <v>94</v>
       </c>
-      <c r="B101" s="26" t="str">
+      <c r="B102" s="26" t="str">
         <f t="shared" si="2"/>
         <v>x5E</v>
       </c>
-      <c r="C101" s="38" t="s">
-        <v>214</v>
-      </c>
-      <c r="D101" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="E101" s="11" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="102" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A102">
+      <c r="C102" s="38" t="s">
+        <v>210</v>
+      </c>
+      <c r="D102" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="E102" s="11" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A103">
         <f t="shared" si="3"/>
         <v>95</v>
       </c>
-      <c r="B102" s="26" t="str">
+      <c r="B103" s="26" t="str">
         <f t="shared" si="2"/>
         <v>x5F</v>
       </c>
-      <c r="C102" s="11" t="s">
-        <v>224</v>
-      </c>
-      <c r="D102" s="5" t="s">
-        <v>236</v>
-      </c>
-      <c r="E102" s="11" t="s">
-        <v>235</v>
-      </c>
-      <c r="F102" s="5" t="s">
+      <c r="C103" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="D103" s="5" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A103">
-        <f t="shared" si="3"/>
-        <v>96</v>
-      </c>
-      <c r="B103" s="26" t="str">
-        <f t="shared" si="2"/>
-        <v>x60</v>
-      </c>
-      <c r="C103" s="42" t="s">
-        <v>227</v>
-      </c>
-      <c r="D103" s="5" t="s">
+      <c r="E103" s="11" t="s">
         <v>231</v>
-      </c>
-      <c r="E103" s="42" t="s">
-        <v>237</v>
       </c>
       <c r="F103" s="5" t="s">
         <v>228</v>
@@ -3116,43 +3194,52 @@
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104">
         <f t="shared" si="3"/>
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B104" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>x61</v>
-      </c>
-      <c r="C104" s="11" t="s">
+        <v>x60</v>
+      </c>
+      <c r="C104" s="42" t="s">
+        <v>223</v>
+      </c>
+      <c r="D104" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="E104" s="42" t="s">
         <v>233</v>
       </c>
-      <c r="D104" s="5" t="s">
-        <v>234</v>
-      </c>
-      <c r="E104" s="11" t="s">
-        <v>238</v>
+      <c r="F104" s="5" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105">
         <f t="shared" si="3"/>
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B105" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>x62</v>
-      </c>
-      <c r="C105" s="11"/>
-      <c r="D105" s="11"/>
-      <c r="E105" s="11"/>
+        <v>x61</v>
+      </c>
+      <c r="C105" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="D105" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="E105" s="11" t="s">
+        <v>234</v>
+      </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106">
         <f t="shared" si="3"/>
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B106" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>x63</v>
+        <v>x62</v>
       </c>
       <c r="C106" s="11"/>
       <c r="D106" s="11"/>
@@ -3161,11 +3248,11 @@
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107">
         <f t="shared" si="3"/>
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B107" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>x64</v>
+        <v>x63</v>
       </c>
       <c r="C107" s="11"/>
       <c r="D107" s="11"/>
@@ -3174,11 +3261,11 @@
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108">
         <f t="shared" si="3"/>
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B108" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>x65</v>
+        <v>x64</v>
       </c>
       <c r="C108" s="11"/>
       <c r="D108" s="11"/>
@@ -3187,235 +3274,232 @@
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109">
         <f t="shared" si="3"/>
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B109" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>x66</v>
-      </c>
+        <v>x65</v>
+      </c>
+      <c r="C109" s="11"/>
+      <c r="D109" s="11"/>
+      <c r="E109" s="11"/>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110">
         <f t="shared" si="3"/>
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B110" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>x67</v>
-      </c>
-      <c r="C110" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="D110" t="s">
-        <v>143</v>
+        <v>x66</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111">
         <f t="shared" si="3"/>
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B111" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>x68</v>
+        <v>x67</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
+      </c>
+      <c r="D111" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112">
         <f t="shared" si="3"/>
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B112" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>x69</v>
+        <v>x68</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113">
         <f t="shared" si="3"/>
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B113" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>x6A</v>
+        <v>x69</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114">
         <f t="shared" si="3"/>
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B114" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>x6B</v>
+        <v>x6A</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115">
         <f t="shared" si="3"/>
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B115" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>x6C</v>
-      </c>
-      <c r="C115" s="30" t="s">
-        <v>118</v>
-      </c>
-      <c r="D115" s="30" t="s">
-        <v>120</v>
-      </c>
-      <c r="E115" s="30" t="s">
-        <v>6</v>
-      </c>
-      <c r="F115" s="5" t="s">
-        <v>119</v>
+        <v>x6B</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116">
         <f t="shared" si="3"/>
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B116" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>x6D</v>
-      </c>
-      <c r="C116" t="s">
-        <v>94</v>
-      </c>
-      <c r="D116" t="s">
-        <v>17</v>
-      </c>
-      <c r="E116" t="s">
-        <v>18</v>
+        <v>x6C</v>
+      </c>
+      <c r="C116" s="30" t="s">
+        <v>118</v>
+      </c>
+      <c r="D116" s="30" t="s">
+        <v>120</v>
+      </c>
+      <c r="E116" s="30" t="s">
+        <v>6</v>
       </c>
       <c r="F116" s="5" t="s">
-        <v>86</v>
+        <v>119</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117">
         <f t="shared" si="3"/>
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B117" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>x6E</v>
-      </c>
-      <c r="C117" s="2" t="s">
-        <v>127</v>
+        <v>x6D</v>
+      </c>
+      <c r="C117" t="s">
+        <v>94</v>
       </c>
       <c r="D117" t="s">
-        <v>126</v>
+        <v>17</v>
+      </c>
+      <c r="E117" t="s">
+        <v>18</v>
       </c>
       <c r="F117" s="5" t="s">
-        <v>165</v>
+        <v>86</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118">
         <f t="shared" si="3"/>
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B118" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>x6F</v>
+        <v>x6E</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D118" t="s">
-        <v>124</v>
+        <v>126</v>
+      </c>
+      <c r="F118" s="5" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119">
         <f t="shared" si="3"/>
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B119" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>x70</v>
+        <v>x6F</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D119" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120">
         <f t="shared" si="3"/>
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B120" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>x71</v>
+        <v>x70</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="D120" s="31" t="s">
+        <v>129</v>
+      </c>
+      <c r="D120" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121">
         <f t="shared" si="3"/>
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B121" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>x72</v>
+        <v>x71</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="D121" t="s">
-        <v>134</v>
+        <v>130</v>
+      </c>
+      <c r="D121" s="31" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122">
         <f t="shared" si="3"/>
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B122" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>x73</v>
+        <v>x72</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="D122" s="31" t="s">
-        <v>125</v>
+        <v>133</v>
+      </c>
+      <c r="D122" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123">
         <f t="shared" si="3"/>
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B123" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>x74</v>
+        <v>x73</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D123" s="31" t="s">
         <v>125</v>
@@ -3424,46 +3508,46 @@
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124">
         <f t="shared" si="3"/>
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B124" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>x75</v>
+        <v>x74</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="D124" t="s">
-        <v>136</v>
+        <v>132</v>
+      </c>
+      <c r="D124" s="31" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125">
         <f t="shared" si="3"/>
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B125" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>x76</v>
+        <v>x75</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="D125" s="31" t="s">
-        <v>125</v>
+        <v>135</v>
+      </c>
+      <c r="D125" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126">
         <f t="shared" si="3"/>
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B126" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>x77</v>
+        <v>x76</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D126" s="31" t="s">
         <v>125</v>
@@ -3472,609 +3556,626 @@
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127">
         <f t="shared" si="3"/>
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B127" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>x78</v>
+        <v>x77</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>146</v>
+        <v>138</v>
+      </c>
+      <c r="D127" s="31" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128">
         <f t="shared" si="3"/>
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B128" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>x79</v>
+        <v>x78</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="D128" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129">
         <f t="shared" si="3"/>
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B129" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>x7A</v>
+        <v>x79</v>
+      </c>
+      <c r="C129" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D129" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130">
         <f t="shared" si="3"/>
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B130" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>x7B</v>
+        <v>x7A</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131">
         <f t="shared" si="3"/>
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B131" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>x7C</v>
-      </c>
-      <c r="C131" s="35"/>
-      <c r="D131" s="35"/>
-      <c r="E131" s="35"/>
-      <c r="F131" s="36"/>
+        <v>x7B</v>
+      </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132">
         <f t="shared" si="3"/>
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B132" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>x7D</v>
-      </c>
+        <v>x7C</v>
+      </c>
+      <c r="C132" s="35"/>
+      <c r="D132" s="35"/>
+      <c r="E132" s="35"/>
+      <c r="F132" s="36"/>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133">
         <f t="shared" si="3"/>
+        <v>125</v>
+      </c>
+      <c r="B133" s="26" t="str">
+        <f t="shared" si="2"/>
+        <v>x7D</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <f t="shared" si="3"/>
         <v>126</v>
       </c>
-      <c r="B133" s="26" t="str">
+      <c r="B134" s="26" t="str">
         <f t="shared" si="2"/>
         <v>x7E</v>
       </c>
-      <c r="C133" t="s">
+      <c r="C134" t="s">
         <v>62</v>
       </c>
-      <c r="D133" t="s">
+      <c r="D134" t="s">
         <v>60</v>
-      </c>
-      <c r="E133" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="134" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A134">
-        <f t="shared" si="3"/>
-        <v>127</v>
-      </c>
-      <c r="B134" s="26" t="str">
-        <f t="shared" si="2"/>
-        <v>x7F</v>
-      </c>
-      <c r="C134" t="s">
-        <v>5</v>
-      </c>
-      <c r="D134" s="5" t="s">
-        <v>73</v>
       </c>
       <c r="E134" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A135">
-        <v>128</v>
+        <f t="shared" si="3"/>
+        <v>127</v>
       </c>
       <c r="B135" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>x80</v>
+        <v>x7F</v>
       </c>
       <c r="C135" t="s">
-        <v>173</v>
-      </c>
-      <c r="D135" t="s">
-        <v>174</v>
+        <v>5</v>
+      </c>
+      <c r="D135" s="5" t="s">
+        <v>73</v>
       </c>
       <c r="E135" t="s">
-        <v>44</v>
+        <v>7</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136">
-        <f>A135+1</f>
+        <v>128</v>
+      </c>
+      <c r="B136" s="26" t="str">
+        <f t="shared" si="2"/>
+        <v>x80</v>
+      </c>
+      <c r="C136" t="s">
+        <v>169</v>
+      </c>
+      <c r="D136" t="s">
+        <v>170</v>
+      </c>
+      <c r="E136" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A137">
+        <f>A136+1</f>
         <v>129</v>
       </c>
-      <c r="B136" s="26" t="str">
-        <f t="shared" ref="B136:B175" si="4">"x" &amp; DEC2HEX(A136,2)</f>
+      <c r="B137" s="26" t="str">
+        <f t="shared" ref="B137:B176" si="4">"x" &amp; DEC2HEX(A137,2)</f>
         <v>x81</v>
       </c>
-      <c r="C136" s="37" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A137" s="37">
-        <f t="shared" ref="A137:A175" si="5">A136+1</f>
+      <c r="C137" s="37" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A138" s="37">
+        <f t="shared" ref="A138:A176" si="5">A137+1</f>
         <v>130</v>
       </c>
-      <c r="B137" s="26" t="str">
+      <c r="B138" s="26" t="str">
         <f t="shared" si="4"/>
         <v>x82</v>
       </c>
-      <c r="C137" s="37" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A138" s="37">
-        <f t="shared" si="5"/>
-        <v>131</v>
-      </c>
-      <c r="B138" s="26" t="str">
-        <f t="shared" si="4"/>
-        <v>x83</v>
-      </c>
       <c r="C138" s="37" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" s="37">
         <f t="shared" si="5"/>
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B139" s="26" t="str">
         <f t="shared" si="4"/>
-        <v>x84</v>
+        <v>x83</v>
       </c>
       <c r="C139" s="37" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" s="37">
         <f t="shared" si="5"/>
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B140" s="26" t="str">
         <f t="shared" si="4"/>
-        <v>x85</v>
+        <v>x84</v>
       </c>
       <c r="C140" s="37" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" s="37">
         <f t="shared" si="5"/>
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B141" s="26" t="str">
         <f t="shared" si="4"/>
-        <v>x86</v>
+        <v>x85</v>
       </c>
       <c r="C141" s="37" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" s="37">
         <f t="shared" si="5"/>
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B142" s="26" t="str">
         <f t="shared" si="4"/>
-        <v>x87</v>
+        <v>x86</v>
       </c>
       <c r="C142" s="37" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" s="37">
         <f t="shared" si="5"/>
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B143" s="26" t="str">
         <f t="shared" si="4"/>
-        <v>x88</v>
+        <v>x87</v>
       </c>
       <c r="C143" s="37" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" s="37">
         <f t="shared" si="5"/>
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B144" s="26" t="str">
         <f t="shared" si="4"/>
-        <v>x89</v>
+        <v>x88</v>
       </c>
       <c r="C144" s="37" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" s="37">
         <f t="shared" si="5"/>
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B145" s="26" t="str">
         <f t="shared" si="4"/>
-        <v>x8A</v>
+        <v>x89</v>
       </c>
       <c r="C145" s="37" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" s="37">
         <f t="shared" si="5"/>
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B146" s="26" t="str">
         <f t="shared" si="4"/>
-        <v>x8B</v>
+        <v>x8A</v>
       </c>
       <c r="C146" s="37" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" s="37">
         <f t="shared" si="5"/>
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B147" s="26" t="str">
         <f t="shared" si="4"/>
-        <v>x8C</v>
+        <v>x8B</v>
       </c>
       <c r="C147" s="37" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" s="37">
         <f t="shared" si="5"/>
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B148" s="26" t="str">
         <f t="shared" si="4"/>
-        <v>x8D</v>
+        <v>x8C</v>
       </c>
       <c r="C148" s="37" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" s="37">
         <f t="shared" si="5"/>
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B149" s="26" t="str">
         <f t="shared" si="4"/>
-        <v>x8E</v>
+        <v>x8D</v>
       </c>
       <c r="C149" s="37" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" s="37">
         <f t="shared" si="5"/>
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B150" s="26" t="str">
         <f t="shared" si="4"/>
-        <v>x8F</v>
+        <v>x8E</v>
       </c>
       <c r="C150" s="37" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" s="37">
         <f t="shared" si="5"/>
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B151" s="26" t="str">
         <f t="shared" si="4"/>
-        <v>x90</v>
+        <v>x8F</v>
       </c>
       <c r="C151" s="37" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" s="37">
         <f t="shared" si="5"/>
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B152" s="26" t="str">
         <f t="shared" si="4"/>
-        <v>x91</v>
+        <v>x90</v>
       </c>
       <c r="C152" s="37" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" s="37">
         <f t="shared" si="5"/>
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B153" s="26" t="str">
         <f t="shared" si="4"/>
-        <v>x92</v>
+        <v>x91</v>
       </c>
       <c r="C153" s="37" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" s="37">
         <f t="shared" si="5"/>
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B154" s="26" t="str">
         <f t="shared" si="4"/>
-        <v>x93</v>
+        <v>x92</v>
       </c>
       <c r="C154" s="37" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" s="37">
         <f t="shared" si="5"/>
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B155" s="26" t="str">
         <f t="shared" si="4"/>
-        <v>x94</v>
+        <v>x93</v>
       </c>
       <c r="C155" s="37" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" s="37">
         <f t="shared" si="5"/>
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B156" s="26" t="str">
         <f t="shared" si="4"/>
-        <v>x95</v>
+        <v>x94</v>
       </c>
       <c r="C156" s="37" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" s="37">
         <f t="shared" si="5"/>
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B157" s="26" t="str">
         <f t="shared" si="4"/>
-        <v>x96</v>
+        <v>x95</v>
       </c>
       <c r="C157" s="37" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" s="37">
         <f t="shared" si="5"/>
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B158" s="26" t="str">
         <f t="shared" si="4"/>
-        <v>x97</v>
+        <v>x96</v>
       </c>
       <c r="C158" s="37" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" s="37">
         <f t="shared" si="5"/>
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B159" s="26" t="str">
         <f t="shared" si="4"/>
-        <v>x98</v>
-      </c>
-      <c r="C159" s="37"/>
+        <v>x97</v>
+      </c>
+      <c r="C159" s="37" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" s="37">
         <f t="shared" si="5"/>
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B160" s="26" t="str">
         <f t="shared" si="4"/>
-        <v>x99</v>
+        <v>x98</v>
       </c>
       <c r="C160" s="37"/>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" s="37">
         <f t="shared" si="5"/>
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B161" s="26" t="str">
         <f t="shared" si="4"/>
-        <v>x9A</v>
-      </c>
-    </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+        <v>x99</v>
+      </c>
+      <c r="C161" s="37"/>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" s="37">
         <f t="shared" si="5"/>
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B162" s="26" t="str">
         <f t="shared" si="4"/>
-        <v>x9B</v>
-      </c>
-    </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+        <v>x9A</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" s="37">
         <f t="shared" si="5"/>
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B163" s="26" t="str">
         <f t="shared" si="4"/>
-        <v>x9C</v>
-      </c>
-    </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+        <v>x9B</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" s="37">
         <f t="shared" si="5"/>
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B164" s="26" t="str">
         <f t="shared" si="4"/>
-        <v>x9D</v>
-      </c>
-    </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+        <v>x9C</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" s="37">
         <f t="shared" si="5"/>
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B165" s="26" t="str">
         <f t="shared" si="4"/>
-        <v>x9E</v>
-      </c>
-    </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+        <v>x9D</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" s="37">
         <f t="shared" si="5"/>
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B166" s="26" t="str">
         <f t="shared" si="4"/>
-        <v>x9F</v>
-      </c>
-    </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+        <v>x9E</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" s="37">
         <f t="shared" si="5"/>
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B167" s="26" t="str">
         <f t="shared" si="4"/>
-        <v>xA0</v>
-      </c>
-    </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+        <v>x9F</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" s="37">
         <f t="shared" si="5"/>
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B168" s="26" t="str">
         <f t="shared" si="4"/>
-        <v>xA1</v>
-      </c>
-    </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+        <v>xA0</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" s="37">
         <f t="shared" si="5"/>
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B169" s="26" t="str">
         <f t="shared" si="4"/>
-        <v>xA2</v>
-      </c>
-    </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+        <v>xA1</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" s="37">
         <f t="shared" si="5"/>
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B170" s="26" t="str">
         <f t="shared" si="4"/>
-        <v>xA3</v>
-      </c>
-    </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+        <v>xA2</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" s="37">
         <f t="shared" si="5"/>
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B171" s="26" t="str">
         <f t="shared" si="4"/>
-        <v>xA4</v>
-      </c>
-    </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+        <v>xA3</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" s="37">
         <f t="shared" si="5"/>
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B172" s="26" t="str">
         <f t="shared" si="4"/>
-        <v>xA5</v>
-      </c>
-    </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+        <v>xA4</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" s="37">
         <f t="shared" si="5"/>
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B173" s="26" t="str">
         <f t="shared" si="4"/>
-        <v>xA6</v>
-      </c>
-    </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+        <v>xA5</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" s="37">
         <f t="shared" si="5"/>
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B174" s="26" t="str">
         <f t="shared" si="4"/>
-        <v>xA7</v>
-      </c>
-    </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+        <v>xA6</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" s="37">
         <f t="shared" si="5"/>
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B175" s="26" t="str">
         <f t="shared" si="4"/>
+        <v>xA7</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A176" s="37">
+        <f t="shared" si="5"/>
+        <v>168</v>
+      </c>
+      <c r="B176" s="26" t="str">
+        <f t="shared" si="4"/>
         <v>xA8</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="A3:E3"/>
     <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
first bits for new array layout
</commit_message>
<xml_diff>
--- a/doc/firmware-register-map.xlsx
+++ b/doc/firmware-register-map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eric\Desktop\projects\beacon\firmware_phased_protoBEACON\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{562CDECB-9F0B-4096-A819-6B4CD2A65585}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A648756-A81C-4957-BFF3-4E30DF3C9140}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26190" yWindow="855" windowWidth="26970" windowHeight="14280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6120" yWindow="1140" windowWidth="21765" windowHeight="13440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1136" uniqueCount="242">
   <si>
     <t>Register Map</t>
   </si>
@@ -811,12 +811,15 @@
       <t>trig_delay defines the delay between rising edge of ext. trig and sending trig to waveform capture. The total delay is given by trig_delay * 128 ns</t>
     </r>
   </si>
+  <si>
+    <t>x000001</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -879,6 +882,13 @@
     <font>
       <strike/>
       <sz val="11"/>
+      <color theme="5" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="5" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -974,7 +984,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1051,13 +1061,14 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1340,8 +1351,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D82" workbookViewId="0">
-      <selection activeCell="F96" sqref="F96"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="D91" sqref="D91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1356,38 +1367,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="45" t="s">
         <v>166</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="44"/>
-      <c r="C3" s="44"/>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
       <c r="F3" s="6"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="45">
+      <c r="A4" s="46">
         <v>43305</v>
       </c>
-      <c r="B4" s="46"/>
+      <c r="B4" s="47"/>
       <c r="C4" s="1"/>
       <c r="D4" t="s">
         <v>168</v>
@@ -1397,11 +1408,11 @@
       </c>
     </row>
     <row r="5" spans="1:7" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="47" t="s">
+      <c r="A5" s="48" t="s">
         <v>235</v>
       </c>
-      <c r="B5" s="47"/>
-      <c r="C5" s="48" t="s">
+      <c r="B5" s="48"/>
+      <c r="C5" s="44" t="s">
         <v>236</v>
       </c>
       <c r="F5" s="5"/>
@@ -3069,8 +3080,8 @@
       <c r="D96" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="E96" s="11" t="s">
-        <v>7</v>
+      <c r="E96" s="49" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>